<commit_message>
Evoked + Heartbeat checking update
</commit_message>
<xml_diff>
--- a/meta/MEG_ANALYSIS_MASTERFILE.xlsx
+++ b/meta/MEG_ANALYSIS_MASTERFILE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\meditation\ERC\Analyses\MEG\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51B6FBD-8051-4675-8EC9-B46D2055717A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536EC4EB-B849-4628-A431-D6B31DCBD3E0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="169">
   <si>
     <t>ANATOMY</t>
   </si>
@@ -527,6 +527,12 @@
   </si>
   <si>
     <t>ico4|6.2</t>
+  </si>
+  <si>
+    <t>MEG</t>
+  </si>
+  <si>
+    <t>bad</t>
   </si>
 </sst>
 </file>
@@ -698,6 +704,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -708,12 +720,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1098,79 +1104,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AY85"/>
+  <dimension ref="A1:AZ85"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
+      <selection pane="bottomRight" activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="C1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="19" t="s">
+      <c r="J1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="19"/>
-      <c r="AH1" s="19"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="19" t="s">
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="21"/>
+      <c r="AE1" s="21"/>
+      <c r="AF1" s="21"/>
+      <c r="AG1" s="21"/>
+      <c r="AH1" s="21"/>
+      <c r="AI1" s="21"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="19"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="19"/>
-      <c r="AP1" s="19"/>
-      <c r="AQ1" s="19"/>
-      <c r="AR1" s="19"/>
-      <c r="AS1" s="19"/>
-      <c r="AT1" s="19"/>
-      <c r="AU1" s="19"/>
-      <c r="AV1" s="19"/>
-      <c r="AW1" s="19"/>
-      <c r="AX1" s="19"/>
-      <c r="AY1" s="19"/>
+      <c r="AL1" s="21"/>
+      <c r="AM1" s="21"/>
+      <c r="AN1" s="21"/>
+      <c r="AO1" s="21"/>
+      <c r="AP1" s="21"/>
+      <c r="AQ1" s="21"/>
+      <c r="AR1" s="21"/>
+      <c r="AS1" s="21"/>
+      <c r="AT1" s="21"/>
+      <c r="AU1" s="21"/>
+      <c r="AV1" s="21"/>
+      <c r="AW1" s="21"/>
+      <c r="AX1" s="21"/>
+      <c r="AY1" s="21"/>
+      <c r="AZ1" s="21"/>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A2" s="17" t="s">
         <v>4</v>
       </c>
@@ -1182,84 +1189,87 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="22"/>
-      <c r="L2" s="23" t="s">
+      <c r="K2" s="18"/>
+      <c r="L2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23" t="s">
+      <c r="M2" s="19"/>
+      <c r="N2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23" t="s">
+      <c r="O2" s="19"/>
+      <c r="P2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
       <c r="S2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="20" t="s">
+      <c r="T2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="4" t="s">
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Z2" s="21" t="s">
+      <c r="AA2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="21"/>
-      <c r="AB2" s="21"/>
-      <c r="AC2" s="21" t="s">
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="AD2" s="21"/>
-      <c r="AE2" s="21"/>
-      <c r="AF2" s="21" t="s">
+      <c r="AE2" s="23"/>
+      <c r="AF2" s="23"/>
+      <c r="AG2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="AG2" s="21"/>
-      <c r="AH2" s="21"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1" t="s">
+      <c r="AH2" s="23"/>
+      <c r="AI2" s="23"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AL2" s="17" t="s">
+      <c r="AM2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="AM2" s="17"/>
-      <c r="AN2" s="1" t="s">
+      <c r="AN2" s="17"/>
+      <c r="AO2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AO2" s="17" t="s">
+      <c r="AP2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="AP2" s="17"/>
       <c r="AQ2" s="17"/>
       <c r="AR2" s="17"/>
-      <c r="AS2" s="17" t="s">
+      <c r="AS2" s="17"/>
+      <c r="AT2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="AT2" s="17"/>
-      <c r="AU2" s="17" t="s">
+      <c r="AU2" s="17"/>
+      <c r="AV2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="AV2" s="17"/>
-      <c r="AW2" s="1"/>
+      <c r="AW2" s="17"/>
       <c r="AX2" s="1"/>
       <c r="AY2" s="1"/>
+      <c r="AZ2" s="1"/>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -1316,20 +1326,20 @@
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
-      <c r="AA3" s="5" t="s">
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AB3" s="5"/>
       <c r="AC3" s="5"/>
-      <c r="AD3" s="5" t="s">
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AE3" s="5"/>
       <c r="AF3" s="5"/>
-      <c r="AG3" s="5" t="s">
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AH3" s="5"/>
       <c r="AI3" s="5"/>
       <c r="AJ3" s="5"/>
       <c r="AK3" s="5"/>
@@ -1347,8 +1357,9 @@
       <c r="AW3" s="5"/>
       <c r="AX3" s="5"/>
       <c r="AY3" s="5"/>
+      <c r="AZ3" s="5"/>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1416,82 +1427,85 @@
       <c r="W4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1" t="s">
+      <c r="X4" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AG4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AG4" s="1" t="s">
+      <c r="AH4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AI4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1" t="s">
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AK4" s="1" t="s">
+      <c r="AL4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AM4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AM4" s="1" t="s">
+      <c r="AN4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AN4" s="1" t="s">
+      <c r="AO4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AO4" s="1" t="s">
+      <c r="AP4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AP4" s="1" t="s">
+      <c r="AQ4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AQ4" s="1" t="s">
+      <c r="AR4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AR4" s="1" t="s">
+      <c r="AS4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AS4" s="1" t="s">
+      <c r="AT4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AT4" s="1" t="s">
+      <c r="AU4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU4" s="1" t="s">
+      <c r="AV4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AV4" s="1" t="s">
+      <c r="AW4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
       <c r="AY4" s="1"/>
+      <c r="AZ4" s="1"/>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>76</v>
       </c>
@@ -1550,20 +1564,20 @@
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
-      <c r="AA5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5">
+        <v>1</v>
+      </c>
       <c r="AC5" s="5"/>
-      <c r="AD5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5">
+        <v>1</v>
+      </c>
       <c r="AF5" s="5"/>
-      <c r="AG5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5">
+        <v>1</v>
+      </c>
       <c r="AI5" s="5"/>
       <c r="AJ5" s="5"/>
       <c r="AK5" s="5"/>
@@ -1581,8 +1595,9 @@
       <c r="AW5" s="5"/>
       <c r="AX5" s="5"/>
       <c r="AY5" s="5"/>
+      <c r="AZ5" s="5"/>
     </row>
-    <row r="6" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>76</v>
       </c>
@@ -1641,20 +1656,20 @@
       <c r="X6" s="9"/>
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
-      <c r="AA6" s="9">
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9">
         <v>-1</v>
       </c>
-      <c r="AB6" s="9"/>
       <c r="AC6" s="9"/>
-      <c r="AD6" s="9">
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9">
         <v>-1</v>
       </c>
-      <c r="AE6" s="9"/>
       <c r="AF6" s="9"/>
-      <c r="AG6" s="9">
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9">
         <v>-1</v>
       </c>
-      <c r="AH6" s="9"/>
       <c r="AI6" s="9"/>
       <c r="AJ6" s="9"/>
       <c r="AK6" s="9"/>
@@ -1672,8 +1687,9 @@
       <c r="AW6" s="9"/>
       <c r="AX6" s="9"/>
       <c r="AY6" s="9"/>
+      <c r="AZ6" s="9"/>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>76</v>
       </c>
@@ -1732,20 +1748,20 @@
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
-      <c r="AA7" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC7" s="5"/>
-      <c r="AD7" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF7" s="5"/>
-      <c r="AG7" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI7" s="5"/>
       <c r="AJ7" s="5"/>
       <c r="AK7" s="5"/>
@@ -1763,8 +1779,9 @@
       <c r="AW7" s="5"/>
       <c r="AX7" s="5"/>
       <c r="AY7" s="5"/>
+      <c r="AZ7" s="5"/>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>76</v>
       </c>
@@ -1823,20 +1840,20 @@
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
-      <c r="AA8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="5">
+        <v>1</v>
+      </c>
       <c r="AC8" s="5"/>
-      <c r="AD8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="5"/>
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="5">
+        <v>1</v>
+      </c>
       <c r="AF8" s="5"/>
-      <c r="AG8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH8" s="5"/>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="5">
+        <v>1</v>
+      </c>
       <c r="AI8" s="5"/>
       <c r="AJ8" s="5"/>
       <c r="AK8" s="5"/>
@@ -1854,8 +1871,9 @@
       <c r="AW8" s="5"/>
       <c r="AX8" s="5"/>
       <c r="AY8" s="5"/>
+      <c r="AZ8" s="5"/>
     </row>
-    <row r="9" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>76</v>
       </c>
@@ -1914,20 +1932,20 @@
       <c r="X9" s="9"/>
       <c r="Y9" s="9"/>
       <c r="Z9" s="9"/>
-      <c r="AA9" s="9">
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9">
         <v>-1</v>
       </c>
-      <c r="AB9" s="9"/>
       <c r="AC9" s="9"/>
-      <c r="AD9" s="9">
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9">
         <v>-1</v>
       </c>
-      <c r="AE9" s="9"/>
       <c r="AF9" s="9"/>
-      <c r="AG9" s="9">
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9">
         <v>-1</v>
       </c>
-      <c r="AH9" s="9"/>
       <c r="AI9" s="9"/>
       <c r="AJ9" s="9"/>
       <c r="AK9" s="9"/>
@@ -1945,8 +1963,9 @@
       <c r="AW9" s="9"/>
       <c r="AX9" s="9"/>
       <c r="AY9" s="9"/>
+      <c r="AZ9" s="9"/>
     </row>
-    <row r="10" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>76</v>
       </c>
@@ -2005,20 +2024,20 @@
       <c r="X10" s="9"/>
       <c r="Y10" s="9"/>
       <c r="Z10" s="9"/>
-      <c r="AA10" s="9">
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9">
         <v>-1</v>
       </c>
-      <c r="AB10" s="9"/>
       <c r="AC10" s="9"/>
-      <c r="AD10" s="9">
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9">
         <v>-1</v>
       </c>
-      <c r="AE10" s="9"/>
       <c r="AF10" s="9"/>
-      <c r="AG10" s="9">
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9">
         <v>-1</v>
       </c>
-      <c r="AH10" s="9"/>
       <c r="AI10" s="9"/>
       <c r="AJ10" s="9"/>
       <c r="AK10" s="9"/>
@@ -2036,8 +2055,9 @@
       <c r="AW10" s="9"/>
       <c r="AX10" s="9"/>
       <c r="AY10" s="9"/>
+      <c r="AZ10" s="9"/>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>76</v>
       </c>
@@ -2096,20 +2116,20 @@
       <c r="X11" s="5"/>
       <c r="Y11" s="5"/>
       <c r="Z11" s="5"/>
-      <c r="AA11" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB11" s="5"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5">
+        <v>1</v>
+      </c>
       <c r="AC11" s="5"/>
-      <c r="AD11" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE11" s="5"/>
+      <c r="AD11" s="5"/>
+      <c r="AE11" s="5">
+        <v>1</v>
+      </c>
       <c r="AF11" s="5"/>
-      <c r="AG11" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH11" s="5"/>
+      <c r="AG11" s="5"/>
+      <c r="AH11" s="5">
+        <v>1</v>
+      </c>
       <c r="AI11" s="5"/>
       <c r="AJ11" s="5"/>
       <c r="AK11" s="5"/>
@@ -2127,8 +2147,9 @@
       <c r="AW11" s="5"/>
       <c r="AX11" s="5"/>
       <c r="AY11" s="5"/>
+      <c r="AZ11" s="5"/>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>76</v>
       </c>
@@ -2187,20 +2208,20 @@
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
       <c r="Z12" s="5"/>
-      <c r="AA12" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="5">
+        <v>1</v>
+      </c>
       <c r="AC12" s="5"/>
-      <c r="AD12" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE12" s="5"/>
+      <c r="AD12" s="5"/>
+      <c r="AE12" s="5">
+        <v>1</v>
+      </c>
       <c r="AF12" s="5"/>
-      <c r="AG12" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH12" s="5"/>
+      <c r="AG12" s="5"/>
+      <c r="AH12" s="5">
+        <v>1</v>
+      </c>
       <c r="AI12" s="5"/>
       <c r="AJ12" s="5"/>
       <c r="AK12" s="5"/>
@@ -2218,8 +2239,9 @@
       <c r="AW12" s="5"/>
       <c r="AX12" s="5"/>
       <c r="AY12" s="5"/>
+      <c r="AZ12" s="5"/>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>76</v>
       </c>
@@ -2278,20 +2300,20 @@
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
-      <c r="AA13" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5">
+        <v>1</v>
+      </c>
       <c r="AC13" s="5"/>
-      <c r="AD13" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE13" s="5"/>
+      <c r="AD13" s="5"/>
+      <c r="AE13" s="5">
+        <v>1</v>
+      </c>
       <c r="AF13" s="5"/>
-      <c r="AG13" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH13" s="5"/>
+      <c r="AG13" s="5"/>
+      <c r="AH13" s="5">
+        <v>1</v>
+      </c>
       <c r="AI13" s="5"/>
       <c r="AJ13" s="5"/>
       <c r="AK13" s="5"/>
@@ -2309,8 +2331,9 @@
       <c r="AW13" s="5"/>
       <c r="AX13" s="5"/>
       <c r="AY13" s="5"/>
+      <c r="AZ13" s="5"/>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>76</v>
       </c>
@@ -2369,20 +2392,20 @@
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
-      <c r="AA14" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC14" s="5"/>
-      <c r="AD14" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF14" s="5"/>
-      <c r="AG14" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH14" s="5"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI14" s="5"/>
       <c r="AJ14" s="5"/>
       <c r="AK14" s="5"/>
@@ -2400,8 +2423,9 @@
       <c r="AW14" s="5"/>
       <c r="AX14" s="5"/>
       <c r="AY14" s="5"/>
+      <c r="AZ14" s="5"/>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>76</v>
       </c>
@@ -2460,20 +2484,20 @@
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
-      <c r="AA15" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5">
+        <v>1</v>
+      </c>
       <c r="AC15" s="5"/>
-      <c r="AD15" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE15" s="5"/>
+      <c r="AD15" s="5"/>
+      <c r="AE15" s="5">
+        <v>1</v>
+      </c>
       <c r="AF15" s="5"/>
-      <c r="AG15" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH15" s="5"/>
+      <c r="AG15" s="5"/>
+      <c r="AH15" s="5">
+        <v>1</v>
+      </c>
       <c r="AI15" s="5"/>
       <c r="AJ15" s="5"/>
       <c r="AK15" s="5"/>
@@ -2491,8 +2515,9 @@
       <c r="AW15" s="5"/>
       <c r="AX15" s="5"/>
       <c r="AY15" s="5"/>
+      <c r="AZ15" s="5"/>
     </row>
-    <row r="16" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>76</v>
       </c>
@@ -2551,20 +2576,20 @@
       <c r="X16" s="11"/>
       <c r="Y16" s="11"/>
       <c r="Z16" s="11"/>
-      <c r="AA16" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11">
+        <v>0</v>
+      </c>
       <c r="AC16" s="11"/>
-      <c r="AD16" s="11">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="11"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="11">
+        <v>0</v>
+      </c>
       <c r="AF16" s="11"/>
-      <c r="AG16" s="11">
-        <v>0</v>
-      </c>
-      <c r="AH16" s="11"/>
+      <c r="AG16" s="11"/>
+      <c r="AH16" s="11">
+        <v>0</v>
+      </c>
       <c r="AI16" s="11"/>
       <c r="AJ16" s="11"/>
       <c r="AK16" s="11"/>
@@ -2582,8 +2607,9 @@
       <c r="AW16" s="11"/>
       <c r="AX16" s="11"/>
       <c r="AY16" s="11"/>
+      <c r="AZ16" s="11"/>
     </row>
-    <row r="17" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>76</v>
       </c>
@@ -2642,20 +2668,20 @@
       <c r="X17" s="11"/>
       <c r="Y17" s="11"/>
       <c r="Z17" s="11"/>
-      <c r="AA17" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11">
+        <v>0</v>
+      </c>
       <c r="AC17" s="11"/>
-      <c r="AD17" s="11">
-        <v>0</v>
-      </c>
-      <c r="AE17" s="11"/>
+      <c r="AD17" s="11"/>
+      <c r="AE17" s="11">
+        <v>0</v>
+      </c>
       <c r="AF17" s="11"/>
-      <c r="AG17" s="11">
-        <v>0</v>
-      </c>
-      <c r="AH17" s="11"/>
+      <c r="AG17" s="11"/>
+      <c r="AH17" s="11">
+        <v>0</v>
+      </c>
       <c r="AI17" s="11"/>
       <c r="AJ17" s="11"/>
       <c r="AK17" s="11"/>
@@ -2673,8 +2699,9 @@
       <c r="AW17" s="11"/>
       <c r="AX17" s="11"/>
       <c r="AY17" s="11"/>
+      <c r="AZ17" s="11"/>
     </row>
-    <row r="18" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>76</v>
       </c>
@@ -2733,20 +2760,20 @@
       <c r="X18" s="11"/>
       <c r="Y18" s="11"/>
       <c r="Z18" s="11"/>
-      <c r="AA18" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AC18" s="11"/>
-      <c r="AD18" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE18" s="11"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AF18" s="11"/>
-      <c r="AG18" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH18" s="11"/>
+      <c r="AG18" s="11"/>
+      <c r="AH18" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AI18" s="11"/>
       <c r="AJ18" s="11"/>
       <c r="AK18" s="11"/>
@@ -2764,8 +2791,9 @@
       <c r="AW18" s="11"/>
       <c r="AX18" s="11"/>
       <c r="AY18" s="11"/>
+      <c r="AZ18" s="11"/>
     </row>
-    <row r="19" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>93</v>
       </c>
@@ -2824,20 +2852,20 @@
       <c r="X19" s="11"/>
       <c r="Y19" s="11"/>
       <c r="Z19" s="11"/>
-      <c r="AA19" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AC19" s="11"/>
-      <c r="AD19" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE19" s="11"/>
+      <c r="AD19" s="11"/>
+      <c r="AE19" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AF19" s="11"/>
-      <c r="AG19" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH19" s="11"/>
+      <c r="AG19" s="11"/>
+      <c r="AH19" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AI19" s="11"/>
       <c r="AJ19" s="11"/>
       <c r="AK19" s="11"/>
@@ -2855,8 +2883,9 @@
       <c r="AW19" s="11"/>
       <c r="AX19" s="11"/>
       <c r="AY19" s="11"/>
+      <c r="AZ19" s="11"/>
     </row>
-    <row r="20" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>76</v>
       </c>
@@ -2915,20 +2944,20 @@
       <c r="X20" s="11"/>
       <c r="Y20" s="11"/>
       <c r="Z20" s="11"/>
-      <c r="AA20" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB20" s="11"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AC20" s="11"/>
-      <c r="AD20" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE20" s="11"/>
+      <c r="AD20" s="11"/>
+      <c r="AE20" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AF20" s="11"/>
-      <c r="AG20" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH20" s="11"/>
+      <c r="AG20" s="11"/>
+      <c r="AH20" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AI20" s="11"/>
       <c r="AJ20" s="11"/>
       <c r="AK20" s="11"/>
@@ -2946,8 +2975,9 @@
       <c r="AW20" s="11"/>
       <c r="AX20" s="11"/>
       <c r="AY20" s="11"/>
+      <c r="AZ20" s="11"/>
     </row>
-    <row r="21" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
         <v>93</v>
       </c>
@@ -3006,20 +3036,20 @@
       <c r="X21" s="11"/>
       <c r="Y21" s="11"/>
       <c r="Z21" s="11"/>
-      <c r="AA21" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB21" s="11"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AC21" s="11"/>
-      <c r="AD21" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE21" s="11"/>
+      <c r="AD21" s="11"/>
+      <c r="AE21" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AF21" s="11"/>
-      <c r="AG21" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH21" s="11"/>
+      <c r="AG21" s="11"/>
+      <c r="AH21" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AI21" s="11"/>
       <c r="AJ21" s="11"/>
       <c r="AK21" s="11"/>
@@ -3037,8 +3067,9 @@
       <c r="AW21" s="11"/>
       <c r="AX21" s="11"/>
       <c r="AY21" s="11"/>
+      <c r="AZ21" s="11"/>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
         <v>76</v>
       </c>
@@ -3097,20 +3128,20 @@
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
-      <c r="AA22" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC22" s="5"/>
-      <c r="AD22" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE22" s="5"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF22" s="5"/>
-      <c r="AG22" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH22" s="5"/>
+      <c r="AG22" s="5"/>
+      <c r="AH22" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI22" s="5"/>
       <c r="AJ22" s="5"/>
       <c r="AK22" s="5"/>
@@ -3128,8 +3159,9 @@
       <c r="AW22" s="5"/>
       <c r="AX22" s="5"/>
       <c r="AY22" s="5"/>
+      <c r="AZ22" s="5"/>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
         <v>76</v>
       </c>
@@ -3188,20 +3220,20 @@
       <c r="X23" s="5"/>
       <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
-      <c r="AA23" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5">
+        <v>1</v>
+      </c>
       <c r="AC23" s="5"/>
-      <c r="AD23" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE23" s="5"/>
+      <c r="AD23" s="5"/>
+      <c r="AE23" s="5">
+        <v>1</v>
+      </c>
       <c r="AF23" s="5"/>
-      <c r="AG23" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH23" s="5"/>
+      <c r="AG23" s="5"/>
+      <c r="AH23" s="5">
+        <v>1</v>
+      </c>
       <c r="AI23" s="5"/>
       <c r="AJ23" s="5"/>
       <c r="AK23" s="5"/>
@@ -3219,8 +3251,9 @@
       <c r="AW23" s="5"/>
       <c r="AX23" s="5"/>
       <c r="AY23" s="5"/>
+      <c r="AZ23" s="5"/>
     </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
         <v>76</v>
       </c>
@@ -3279,20 +3312,20 @@
       <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
-      <c r="AA24" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB24" s="5"/>
+      <c r="AA24" s="5"/>
+      <c r="AB24" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC24" s="5"/>
-      <c r="AD24" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE24" s="5"/>
+      <c r="AD24" s="5"/>
+      <c r="AE24" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF24" s="5"/>
-      <c r="AG24" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH24" s="5"/>
+      <c r="AG24" s="5"/>
+      <c r="AH24" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI24" s="5"/>
       <c r="AJ24" s="5"/>
       <c r="AK24" s="5"/>
@@ -3310,8 +3343,9 @@
       <c r="AW24" s="5"/>
       <c r="AX24" s="5"/>
       <c r="AY24" s="5"/>
+      <c r="AZ24" s="5"/>
     </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
         <v>76</v>
       </c>
@@ -3370,20 +3404,20 @@
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
-      <c r="AA25" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB25" s="5"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="5">
+        <v>1</v>
+      </c>
       <c r="AC25" s="5"/>
-      <c r="AD25" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE25" s="5"/>
+      <c r="AD25" s="5"/>
+      <c r="AE25" s="5">
+        <v>1</v>
+      </c>
       <c r="AF25" s="5"/>
-      <c r="AG25" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH25" s="5"/>
+      <c r="AG25" s="5"/>
+      <c r="AH25" s="5">
+        <v>1</v>
+      </c>
       <c r="AI25" s="5"/>
       <c r="AJ25" s="5"/>
       <c r="AK25" s="5"/>
@@ -3401,8 +3435,9 @@
       <c r="AW25" s="5"/>
       <c r="AX25" s="5"/>
       <c r="AY25" s="5"/>
+      <c r="AZ25" s="5"/>
     </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A26" s="5" t="s">
         <v>76</v>
       </c>
@@ -3461,20 +3496,20 @@
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
       <c r="Z26" s="5"/>
-      <c r="AA26" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB26" s="5"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="5">
+        <v>1</v>
+      </c>
       <c r="AC26" s="5"/>
-      <c r="AD26" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE26" s="5"/>
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5">
+        <v>1</v>
+      </c>
       <c r="AF26" s="5"/>
-      <c r="AG26" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH26" s="5"/>
+      <c r="AG26" s="5"/>
+      <c r="AH26" s="5">
+        <v>1</v>
+      </c>
       <c r="AI26" s="5"/>
       <c r="AJ26" s="5"/>
       <c r="AK26" s="5"/>
@@ -3492,8 +3527,9 @@
       <c r="AW26" s="5"/>
       <c r="AX26" s="5"/>
       <c r="AY26" s="5"/>
+      <c r="AZ26" s="5"/>
     </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A27" s="5" t="s">
         <v>76</v>
       </c>
@@ -3552,20 +3588,20 @@
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
-      <c r="AA27" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC27" s="5"/>
-      <c r="AD27" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE27" s="5"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF27" s="5"/>
-      <c r="AG27" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH27" s="5"/>
+      <c r="AG27" s="5"/>
+      <c r="AH27" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI27" s="5"/>
       <c r="AJ27" s="5"/>
       <c r="AK27" s="5"/>
@@ -3583,8 +3619,9 @@
       <c r="AW27" s="5"/>
       <c r="AX27" s="5"/>
       <c r="AY27" s="5"/>
+      <c r="AZ27" s="5"/>
     </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A28" s="5" t="s">
         <v>76</v>
       </c>
@@ -3643,20 +3680,20 @@
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
       <c r="Z28" s="5"/>
-      <c r="AA28" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC28" s="5"/>
-      <c r="AD28" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE28" s="5"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF28" s="5"/>
-      <c r="AG28" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH28" s="5"/>
+      <c r="AG28" s="5"/>
+      <c r="AH28" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI28" s="5"/>
       <c r="AJ28" s="5"/>
       <c r="AK28" s="5"/>
@@ -3674,8 +3711,9 @@
       <c r="AW28" s="5"/>
       <c r="AX28" s="5"/>
       <c r="AY28" s="5"/>
+      <c r="AZ28" s="5"/>
     </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
         <v>76</v>
       </c>
@@ -3734,20 +3772,20 @@
       <c r="X29" s="5"/>
       <c r="Y29" s="5"/>
       <c r="Z29" s="5"/>
-      <c r="AA29" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB29" s="5"/>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC29" s="5"/>
-      <c r="AD29" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE29" s="5"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF29" s="5"/>
-      <c r="AG29" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH29" s="5"/>
+      <c r="AG29" s="5"/>
+      <c r="AH29" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI29" s="5"/>
       <c r="AJ29" s="5"/>
       <c r="AK29" s="5"/>
@@ -3765,8 +3803,9 @@
       <c r="AW29" s="5"/>
       <c r="AX29" s="5"/>
       <c r="AY29" s="5"/>
+      <c r="AZ29" s="5"/>
     </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
         <v>76</v>
       </c>
@@ -3825,20 +3864,20 @@
       <c r="X30" s="5"/>
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
-      <c r="AA30" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB30" s="5"/>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="5">
+        <v>1</v>
+      </c>
       <c r="AC30" s="5"/>
-      <c r="AD30" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE30" s="5"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="5">
+        <v>1</v>
+      </c>
       <c r="AF30" s="5"/>
-      <c r="AG30" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH30" s="5"/>
+      <c r="AG30" s="5"/>
+      <c r="AH30" s="5">
+        <v>1</v>
+      </c>
       <c r="AI30" s="5"/>
       <c r="AJ30" s="5"/>
       <c r="AK30" s="5"/>
@@ -3856,8 +3895,9 @@
       <c r="AW30" s="5"/>
       <c r="AX30" s="5"/>
       <c r="AY30" s="5"/>
+      <c r="AZ30" s="5"/>
     </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
         <v>76</v>
       </c>
@@ -3916,20 +3956,20 @@
       <c r="X31" s="5"/>
       <c r="Y31" s="5"/>
       <c r="Z31" s="5"/>
-      <c r="AA31" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB31" s="5"/>
+      <c r="AA31" s="5"/>
+      <c r="AB31" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC31" s="5"/>
-      <c r="AD31" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE31" s="5"/>
+      <c r="AD31" s="5"/>
+      <c r="AE31" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF31" s="5"/>
-      <c r="AG31" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH31" s="5"/>
+      <c r="AG31" s="5"/>
+      <c r="AH31" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI31" s="5"/>
       <c r="AJ31" s="5"/>
       <c r="AK31" s="5"/>
@@ -3947,8 +3987,9 @@
       <c r="AW31" s="5"/>
       <c r="AX31" s="5"/>
       <c r="AY31" s="5"/>
+      <c r="AZ31" s="5"/>
     </row>
-    <row r="32" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A32" s="11" t="s">
         <v>76</v>
       </c>
@@ -4007,20 +4048,20 @@
       <c r="X32" s="11"/>
       <c r="Y32" s="11"/>
       <c r="Z32" s="11"/>
-      <c r="AA32" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB32" s="11"/>
+      <c r="AA32" s="11"/>
+      <c r="AB32" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AC32" s="11"/>
-      <c r="AD32" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE32" s="11"/>
+      <c r="AD32" s="11"/>
+      <c r="AE32" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AF32" s="11"/>
-      <c r="AG32" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH32" s="11"/>
+      <c r="AG32" s="11"/>
+      <c r="AH32" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AI32" s="11"/>
       <c r="AJ32" s="11"/>
       <c r="AK32" s="11"/>
@@ -4038,8 +4079,9 @@
       <c r="AW32" s="11"/>
       <c r="AX32" s="11"/>
       <c r="AY32" s="11"/>
+      <c r="AZ32" s="11"/>
     </row>
-    <row r="33" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>76</v>
       </c>
@@ -4098,20 +4140,20 @@
       <c r="X33" s="9"/>
       <c r="Y33" s="9"/>
       <c r="Z33" s="9"/>
-      <c r="AA33" s="9">
+      <c r="AA33" s="9"/>
+      <c r="AB33" s="9">
         <v>-1</v>
       </c>
-      <c r="AB33" s="9"/>
       <c r="AC33" s="9"/>
-      <c r="AD33" s="9">
+      <c r="AD33" s="9"/>
+      <c r="AE33" s="9">
         <v>-1</v>
       </c>
-      <c r="AE33" s="9"/>
       <c r="AF33" s="9"/>
-      <c r="AG33" s="9">
+      <c r="AG33" s="9"/>
+      <c r="AH33" s="9">
         <v>-1</v>
       </c>
-      <c r="AH33" s="9"/>
       <c r="AI33" s="9"/>
       <c r="AJ33" s="9"/>
       <c r="AK33" s="9"/>
@@ -4129,8 +4171,9 @@
       <c r="AW33" s="9"/>
       <c r="AX33" s="9"/>
       <c r="AY33" s="9"/>
+      <c r="AZ33" s="9"/>
     </row>
-    <row r="34" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A34" s="5" t="s">
         <v>76</v>
       </c>
@@ -4189,20 +4232,20 @@
       <c r="X34" s="5"/>
       <c r="Y34" s="5"/>
       <c r="Z34" s="5"/>
-      <c r="AA34" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB34" s="5"/>
+      <c r="AA34" s="5"/>
+      <c r="AB34" s="5">
+        <v>1</v>
+      </c>
       <c r="AC34" s="5"/>
-      <c r="AD34" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE34" s="5"/>
+      <c r="AD34" s="5"/>
+      <c r="AE34" s="5">
+        <v>1</v>
+      </c>
       <c r="AF34" s="5"/>
-      <c r="AG34" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH34" s="5"/>
+      <c r="AG34" s="5"/>
+      <c r="AH34" s="5">
+        <v>1</v>
+      </c>
       <c r="AI34" s="5"/>
       <c r="AJ34" s="5"/>
       <c r="AK34" s="5"/>
@@ -4220,8 +4263,9 @@
       <c r="AW34" s="5"/>
       <c r="AX34" s="5"/>
       <c r="AY34" s="5"/>
+      <c r="AZ34" s="5"/>
     </row>
-    <row r="35" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
         <v>93</v>
       </c>
@@ -4279,20 +4323,20 @@
       <c r="X35" s="5"/>
       <c r="Y35" s="5"/>
       <c r="Z35" s="5"/>
-      <c r="AA35" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB35" s="5"/>
+      <c r="AA35" s="5"/>
+      <c r="AB35" s="5">
+        <v>1</v>
+      </c>
       <c r="AC35" s="5"/>
-      <c r="AD35" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE35" s="5"/>
+      <c r="AD35" s="5"/>
+      <c r="AE35" s="5">
+        <v>1</v>
+      </c>
       <c r="AF35" s="5"/>
-      <c r="AG35" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH35" s="5"/>
+      <c r="AG35" s="5"/>
+      <c r="AH35" s="5">
+        <v>1</v>
+      </c>
       <c r="AI35" s="5"/>
       <c r="AJ35" s="5"/>
       <c r="AK35" s="5"/>
@@ -4310,8 +4354,9 @@
       <c r="AW35" s="5"/>
       <c r="AX35" s="5"/>
       <c r="AY35" s="5"/>
+      <c r="AZ35" s="5"/>
     </row>
-    <row r="36" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A36" s="11" t="s">
         <v>93</v>
       </c>
@@ -4370,20 +4415,20 @@
       <c r="X36" s="11"/>
       <c r="Y36" s="11"/>
       <c r="Z36" s="11"/>
-      <c r="AA36" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB36" s="11"/>
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AC36" s="11"/>
-      <c r="AD36" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE36" s="11"/>
+      <c r="AD36" s="11"/>
+      <c r="AE36" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AF36" s="11"/>
-      <c r="AG36" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH36" s="11"/>
+      <c r="AG36" s="11"/>
+      <c r="AH36" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AI36" s="11"/>
       <c r="AJ36" s="11"/>
       <c r="AK36" s="11"/>
@@ -4401,8 +4446,9 @@
       <c r="AW36" s="11"/>
       <c r="AX36" s="11"/>
       <c r="AY36" s="11"/>
+      <c r="AZ36" s="11"/>
     </row>
-    <row r="37" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
         <v>93</v>
       </c>
@@ -4461,20 +4507,20 @@
       <c r="X37" s="5"/>
       <c r="Y37" s="5"/>
       <c r="Z37" s="5"/>
-      <c r="AA37" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB37" s="5"/>
+      <c r="AA37" s="5"/>
+      <c r="AB37" s="5">
+        <v>1</v>
+      </c>
       <c r="AC37" s="5"/>
-      <c r="AD37" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE37" s="5"/>
+      <c r="AD37" s="5"/>
+      <c r="AE37" s="5">
+        <v>1</v>
+      </c>
       <c r="AF37" s="5"/>
-      <c r="AG37" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH37" s="5"/>
+      <c r="AG37" s="5"/>
+      <c r="AH37" s="5">
+        <v>1</v>
+      </c>
       <c r="AI37" s="5"/>
       <c r="AJ37" s="5"/>
       <c r="AK37" s="5"/>
@@ -4492,8 +4538,9 @@
       <c r="AW37" s="5"/>
       <c r="AX37" s="5"/>
       <c r="AY37" s="5"/>
+      <c r="AZ37" s="5"/>
     </row>
-    <row r="38" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A38" s="5" t="s">
         <v>93</v>
       </c>
@@ -4552,20 +4599,20 @@
       <c r="X38" s="5"/>
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
-      <c r="AA38" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB38" s="5"/>
+      <c r="AA38" s="5"/>
+      <c r="AB38" s="5">
+        <v>1</v>
+      </c>
       <c r="AC38" s="5"/>
-      <c r="AD38" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE38" s="5"/>
+      <c r="AD38" s="5"/>
+      <c r="AE38" s="5">
+        <v>1</v>
+      </c>
       <c r="AF38" s="5"/>
-      <c r="AG38" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH38" s="5"/>
+      <c r="AG38" s="5"/>
+      <c r="AH38" s="5">
+        <v>1</v>
+      </c>
       <c r="AI38" s="5"/>
       <c r="AJ38" s="5"/>
       <c r="AK38" s="5"/>
@@ -4583,8 +4630,9 @@
       <c r="AW38" s="5"/>
       <c r="AX38" s="5"/>
       <c r="AY38" s="5"/>
+      <c r="AZ38" s="5"/>
     </row>
-    <row r="39" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A39" s="5" t="s">
         <v>93</v>
       </c>
@@ -4643,20 +4691,20 @@
       <c r="X39" s="5"/>
       <c r="Y39" s="5"/>
       <c r="Z39" s="5"/>
-      <c r="AA39" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB39" s="5"/>
+      <c r="AA39" s="5"/>
+      <c r="AB39" s="5">
+        <v>1</v>
+      </c>
       <c r="AC39" s="5"/>
-      <c r="AD39" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE39" s="5"/>
+      <c r="AD39" s="5"/>
+      <c r="AE39" s="5">
+        <v>1</v>
+      </c>
       <c r="AF39" s="5"/>
-      <c r="AG39" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH39" s="5"/>
+      <c r="AG39" s="5"/>
+      <c r="AH39" s="5">
+        <v>1</v>
+      </c>
       <c r="AI39" s="5"/>
       <c r="AJ39" s="5"/>
       <c r="AK39" s="5"/>
@@ -4674,8 +4722,9 @@
       <c r="AW39" s="5"/>
       <c r="AX39" s="5"/>
       <c r="AY39" s="5"/>
+      <c r="AZ39" s="5"/>
     </row>
-    <row r="40" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A40" s="5" t="s">
         <v>93</v>
       </c>
@@ -4734,20 +4783,20 @@
       <c r="X40" s="5"/>
       <c r="Y40" s="5"/>
       <c r="Z40" s="5"/>
-      <c r="AA40" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB40" s="5"/>
+      <c r="AA40" s="5"/>
+      <c r="AB40" s="5">
+        <v>1</v>
+      </c>
       <c r="AC40" s="5"/>
-      <c r="AD40" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE40" s="5"/>
+      <c r="AD40" s="5"/>
+      <c r="AE40" s="5">
+        <v>1</v>
+      </c>
       <c r="AF40" s="5"/>
-      <c r="AG40" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH40" s="5"/>
+      <c r="AG40" s="5"/>
+      <c r="AH40" s="5">
+        <v>1</v>
+      </c>
       <c r="AI40" s="5"/>
       <c r="AJ40" s="5"/>
       <c r="AK40" s="5"/>
@@ -4765,8 +4814,9 @@
       <c r="AW40" s="5"/>
       <c r="AX40" s="5"/>
       <c r="AY40" s="5"/>
+      <c r="AZ40" s="5"/>
     </row>
-    <row r="41" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A41" s="5" t="s">
         <v>93</v>
       </c>
@@ -4825,20 +4875,20 @@
       <c r="X41" s="5"/>
       <c r="Y41" s="5"/>
       <c r="Z41" s="5"/>
-      <c r="AA41" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB41" s="5"/>
+      <c r="AA41" s="5"/>
+      <c r="AB41" s="5">
+        <v>1</v>
+      </c>
       <c r="AC41" s="5"/>
-      <c r="AD41" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE41" s="5"/>
+      <c r="AD41" s="5"/>
+      <c r="AE41" s="5">
+        <v>1</v>
+      </c>
       <c r="AF41" s="5"/>
-      <c r="AG41" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH41" s="5"/>
+      <c r="AG41" s="5"/>
+      <c r="AH41" s="5">
+        <v>1</v>
+      </c>
       <c r="AI41" s="5"/>
       <c r="AJ41" s="5"/>
       <c r="AK41" s="5"/>
@@ -4856,8 +4906,9 @@
       <c r="AW41" s="5"/>
       <c r="AX41" s="5"/>
       <c r="AY41" s="5"/>
+      <c r="AZ41" s="5"/>
     </row>
-    <row r="42" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A42" s="5" t="s">
         <v>93</v>
       </c>
@@ -4916,20 +4967,20 @@
       <c r="X42" s="5"/>
       <c r="Y42" s="5"/>
       <c r="Z42" s="5"/>
-      <c r="AA42" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB42" s="5"/>
+      <c r="AA42" s="5"/>
+      <c r="AB42" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC42" s="5"/>
-      <c r="AD42" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE42" s="5"/>
+      <c r="AD42" s="5"/>
+      <c r="AE42" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF42" s="5"/>
-      <c r="AG42" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH42" s="5"/>
+      <c r="AG42" s="5"/>
+      <c r="AH42" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI42" s="5"/>
       <c r="AJ42" s="5"/>
       <c r="AK42" s="5"/>
@@ -4947,8 +4998,9 @@
       <c r="AW42" s="5"/>
       <c r="AX42" s="5"/>
       <c r="AY42" s="5"/>
+      <c r="AZ42" s="5"/>
     </row>
-    <row r="43" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A43" s="5" t="s">
         <v>93</v>
       </c>
@@ -5007,20 +5059,20 @@
       <c r="X43" s="5"/>
       <c r="Y43" s="5"/>
       <c r="Z43" s="5"/>
-      <c r="AA43" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB43" s="5"/>
+      <c r="AA43" s="5"/>
+      <c r="AB43" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC43" s="5"/>
-      <c r="AD43" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE43" s="5"/>
+      <c r="AD43" s="5"/>
+      <c r="AE43" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF43" s="5"/>
-      <c r="AG43" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH43" s="5"/>
+      <c r="AG43" s="5"/>
+      <c r="AH43" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI43" s="5"/>
       <c r="AJ43" s="5"/>
       <c r="AK43" s="5"/>
@@ -5038,8 +5090,9 @@
       <c r="AW43" s="5"/>
       <c r="AX43" s="5"/>
       <c r="AY43" s="5"/>
+      <c r="AZ43" s="5"/>
     </row>
-    <row r="44" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A44" s="5" t="s">
         <v>93</v>
       </c>
@@ -5098,20 +5151,20 @@
       <c r="X44" s="5"/>
       <c r="Y44" s="5"/>
       <c r="Z44" s="5"/>
-      <c r="AA44" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB44" s="5"/>
+      <c r="AA44" s="5"/>
+      <c r="AB44" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC44" s="5"/>
-      <c r="AD44" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE44" s="5"/>
+      <c r="AD44" s="5"/>
+      <c r="AE44" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF44" s="5"/>
-      <c r="AG44" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH44" s="5"/>
+      <c r="AG44" s="5"/>
+      <c r="AH44" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI44" s="5"/>
       <c r="AJ44" s="5"/>
       <c r="AK44" s="5"/>
@@ -5129,8 +5182,9 @@
       <c r="AW44" s="5"/>
       <c r="AX44" s="5"/>
       <c r="AY44" s="5"/>
+      <c r="AZ44" s="5"/>
     </row>
-    <row r="45" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A45" s="5" t="s">
         <v>93</v>
       </c>
@@ -5189,20 +5243,20 @@
       <c r="X45" s="5"/>
       <c r="Y45" s="5"/>
       <c r="Z45" s="5"/>
-      <c r="AA45" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB45" s="5"/>
+      <c r="AA45" s="5"/>
+      <c r="AB45" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC45" s="5"/>
-      <c r="AD45" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE45" s="5"/>
+      <c r="AD45" s="5"/>
+      <c r="AE45" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF45" s="5"/>
-      <c r="AG45" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH45" s="5"/>
+      <c r="AG45" s="5"/>
+      <c r="AH45" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI45" s="5"/>
       <c r="AJ45" s="5"/>
       <c r="AK45" s="5"/>
@@ -5220,8 +5274,9 @@
       <c r="AW45" s="5"/>
       <c r="AX45" s="5"/>
       <c r="AY45" s="5"/>
+      <c r="AZ45" s="5"/>
     </row>
-    <row r="46" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A46" s="5" t="s">
         <v>93</v>
       </c>
@@ -5280,20 +5335,20 @@
       <c r="X46" s="5"/>
       <c r="Y46" s="5"/>
       <c r="Z46" s="5"/>
-      <c r="AA46" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB46" s="5"/>
+      <c r="AA46" s="5"/>
+      <c r="AB46" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC46" s="5"/>
-      <c r="AD46" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE46" s="5"/>
+      <c r="AD46" s="5"/>
+      <c r="AE46" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF46" s="5"/>
-      <c r="AG46" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH46" s="5"/>
+      <c r="AG46" s="5"/>
+      <c r="AH46" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI46" s="5"/>
       <c r="AJ46" s="5"/>
       <c r="AK46" s="5"/>
@@ -5311,8 +5366,9 @@
       <c r="AW46" s="5"/>
       <c r="AX46" s="5"/>
       <c r="AY46" s="5"/>
+      <c r="AZ46" s="5"/>
     </row>
-    <row r="47" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A47" s="5" t="s">
         <v>93</v>
       </c>
@@ -5371,20 +5427,20 @@
       <c r="X47" s="5"/>
       <c r="Y47" s="5"/>
       <c r="Z47" s="5"/>
-      <c r="AA47" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB47" s="5"/>
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="5">
+        <v>1</v>
+      </c>
       <c r="AC47" s="5"/>
-      <c r="AD47" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE47" s="5"/>
+      <c r="AD47" s="5"/>
+      <c r="AE47" s="5">
+        <v>1</v>
+      </c>
       <c r="AF47" s="5"/>
-      <c r="AG47" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH47" s="5"/>
+      <c r="AG47" s="5"/>
+      <c r="AH47" s="5">
+        <v>1</v>
+      </c>
       <c r="AI47" s="5"/>
       <c r="AJ47" s="5"/>
       <c r="AK47" s="5"/>
@@ -5402,8 +5458,9 @@
       <c r="AW47" s="5"/>
       <c r="AX47" s="5"/>
       <c r="AY47" s="5"/>
+      <c r="AZ47" s="5"/>
     </row>
-    <row r="48" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A48" s="5" t="s">
         <v>93</v>
       </c>
@@ -5462,20 +5519,20 @@
       <c r="X48" s="5"/>
       <c r="Y48" s="5"/>
       <c r="Z48" s="5"/>
-      <c r="AA48" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB48" s="5"/>
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="5">
+        <v>1</v>
+      </c>
       <c r="AC48" s="5"/>
-      <c r="AD48" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE48" s="5"/>
+      <c r="AD48" s="5"/>
+      <c r="AE48" s="5">
+        <v>1</v>
+      </c>
       <c r="AF48" s="5"/>
-      <c r="AG48" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH48" s="5"/>
+      <c r="AG48" s="5"/>
+      <c r="AH48" s="5">
+        <v>1</v>
+      </c>
       <c r="AI48" s="5"/>
       <c r="AJ48" s="5"/>
       <c r="AK48" s="5"/>
@@ -5493,8 +5550,9 @@
       <c r="AW48" s="5"/>
       <c r="AX48" s="5"/>
       <c r="AY48" s="5"/>
+      <c r="AZ48" s="5"/>
     </row>
-    <row r="49" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A49" s="11" t="s">
         <v>93</v>
       </c>
@@ -5553,20 +5611,20 @@
       <c r="X49" s="11"/>
       <c r="Y49" s="11"/>
       <c r="Z49" s="11"/>
-      <c r="AA49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB49" s="11"/>
+      <c r="AA49" s="11"/>
+      <c r="AB49" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AC49" s="11"/>
-      <c r="AD49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE49" s="11"/>
+      <c r="AD49" s="11"/>
+      <c r="AE49" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AF49" s="11"/>
-      <c r="AG49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH49" s="11"/>
+      <c r="AG49" s="11"/>
+      <c r="AH49" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AI49" s="11"/>
       <c r="AJ49" s="11"/>
       <c r="AK49" s="11"/>
@@ -5584,8 +5642,9 @@
       <c r="AW49" s="11"/>
       <c r="AX49" s="11"/>
       <c r="AY49" s="11"/>
+      <c r="AZ49" s="11"/>
     </row>
-    <row r="50" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A50" s="5" t="s">
         <v>93</v>
       </c>
@@ -5644,20 +5703,20 @@
       <c r="X50" s="5"/>
       <c r="Y50" s="5"/>
       <c r="Z50" s="5"/>
-      <c r="AA50" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB50" s="5"/>
+      <c r="AA50" s="5"/>
+      <c r="AB50" s="5">
+        <v>1</v>
+      </c>
       <c r="AC50" s="5"/>
-      <c r="AD50" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE50" s="5"/>
+      <c r="AD50" s="5"/>
+      <c r="AE50" s="5">
+        <v>1</v>
+      </c>
       <c r="AF50" s="5"/>
-      <c r="AG50" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH50" s="5"/>
+      <c r="AG50" s="5"/>
+      <c r="AH50" s="5">
+        <v>1</v>
+      </c>
       <c r="AI50" s="5"/>
       <c r="AJ50" s="5"/>
       <c r="AK50" s="5"/>
@@ -5675,8 +5734,9 @@
       <c r="AW50" s="5"/>
       <c r="AX50" s="5"/>
       <c r="AY50" s="5"/>
+      <c r="AZ50" s="5"/>
     </row>
-    <row r="51" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A51" s="5" t="s">
         <v>93</v>
       </c>
@@ -5735,20 +5795,20 @@
       <c r="X51" s="5"/>
       <c r="Y51" s="5"/>
       <c r="Z51" s="5"/>
-      <c r="AA51" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB51" s="5"/>
+      <c r="AA51" s="5"/>
+      <c r="AB51" s="5">
+        <v>1</v>
+      </c>
       <c r="AC51" s="5"/>
-      <c r="AD51" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE51" s="5"/>
+      <c r="AD51" s="5"/>
+      <c r="AE51" s="5">
+        <v>1</v>
+      </c>
       <c r="AF51" s="5"/>
-      <c r="AG51" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH51" s="5"/>
+      <c r="AG51" s="5"/>
+      <c r="AH51" s="5">
+        <v>1</v>
+      </c>
       <c r="AI51" s="5"/>
       <c r="AJ51" s="5"/>
       <c r="AK51" s="5"/>
@@ -5766,8 +5826,9 @@
       <c r="AW51" s="5"/>
       <c r="AX51" s="5"/>
       <c r="AY51" s="5"/>
+      <c r="AZ51" s="5"/>
     </row>
-    <row r="52" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A52" s="5" t="s">
         <v>93</v>
       </c>
@@ -5826,20 +5887,20 @@
       <c r="X52" s="5"/>
       <c r="Y52" s="5"/>
       <c r="Z52" s="5"/>
-      <c r="AA52" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB52" s="5"/>
+      <c r="AA52" s="5"/>
+      <c r="AB52" s="5">
+        <v>1</v>
+      </c>
       <c r="AC52" s="5"/>
-      <c r="AD52" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE52" s="5"/>
+      <c r="AD52" s="5"/>
+      <c r="AE52" s="5">
+        <v>1</v>
+      </c>
       <c r="AF52" s="5"/>
-      <c r="AG52" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH52" s="5"/>
+      <c r="AG52" s="5"/>
+      <c r="AH52" s="5">
+        <v>1</v>
+      </c>
       <c r="AI52" s="5"/>
       <c r="AJ52" s="5"/>
       <c r="AK52" s="5"/>
@@ -5857,8 +5918,9 @@
       <c r="AW52" s="5"/>
       <c r="AX52" s="5"/>
       <c r="AY52" s="5"/>
+      <c r="AZ52" s="5"/>
     </row>
-    <row r="53" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A53" s="5" t="s">
         <v>93</v>
       </c>
@@ -5917,20 +5979,20 @@
       <c r="X53" s="5"/>
       <c r="Y53" s="5"/>
       <c r="Z53" s="5"/>
-      <c r="AA53" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB53" s="5"/>
+      <c r="AA53" s="5"/>
+      <c r="AB53" s="5">
+        <v>1</v>
+      </c>
       <c r="AC53" s="5"/>
-      <c r="AD53" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE53" s="5"/>
+      <c r="AD53" s="5"/>
+      <c r="AE53" s="5">
+        <v>1</v>
+      </c>
       <c r="AF53" s="5"/>
-      <c r="AG53" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH53" s="5"/>
+      <c r="AG53" s="5"/>
+      <c r="AH53" s="5">
+        <v>1</v>
+      </c>
       <c r="AI53" s="5"/>
       <c r="AJ53" s="5"/>
       <c r="AK53" s="5"/>
@@ -5948,8 +6010,9 @@
       <c r="AW53" s="5"/>
       <c r="AX53" s="5"/>
       <c r="AY53" s="5"/>
+      <c r="AZ53" s="5"/>
     </row>
-    <row r="54" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A54" s="5" t="s">
         <v>93</v>
       </c>
@@ -6008,20 +6071,20 @@
       <c r="X54" s="5"/>
       <c r="Y54" s="5"/>
       <c r="Z54" s="5"/>
-      <c r="AA54" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB54" s="5"/>
+      <c r="AA54" s="5"/>
+      <c r="AB54" s="5">
+        <v>1</v>
+      </c>
       <c r="AC54" s="5"/>
-      <c r="AD54" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE54" s="5"/>
+      <c r="AD54" s="5"/>
+      <c r="AE54" s="5">
+        <v>1</v>
+      </c>
       <c r="AF54" s="5"/>
-      <c r="AG54" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH54" s="5"/>
+      <c r="AG54" s="5"/>
+      <c r="AH54" s="5">
+        <v>1</v>
+      </c>
       <c r="AI54" s="5"/>
       <c r="AJ54" s="5"/>
       <c r="AK54" s="5"/>
@@ -6039,8 +6102,9 @@
       <c r="AW54" s="5"/>
       <c r="AX54" s="5"/>
       <c r="AY54" s="5"/>
+      <c r="AZ54" s="5"/>
     </row>
-    <row r="55" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A55" s="5" t="s">
         <v>93</v>
       </c>
@@ -6099,20 +6163,20 @@
       <c r="X55" s="5"/>
       <c r="Y55" s="5"/>
       <c r="Z55" s="5"/>
-      <c r="AA55" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB55" s="5"/>
+      <c r="AA55" s="5"/>
+      <c r="AB55" s="5">
+        <v>1</v>
+      </c>
       <c r="AC55" s="5"/>
-      <c r="AD55" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE55" s="5"/>
+      <c r="AD55" s="5"/>
+      <c r="AE55" s="5">
+        <v>1</v>
+      </c>
       <c r="AF55" s="5"/>
-      <c r="AG55" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH55" s="5"/>
+      <c r="AG55" s="5"/>
+      <c r="AH55" s="5">
+        <v>1</v>
+      </c>
       <c r="AI55" s="5"/>
       <c r="AJ55" s="5"/>
       <c r="AK55" s="5"/>
@@ -6130,8 +6194,9 @@
       <c r="AW55" s="5"/>
       <c r="AX55" s="5"/>
       <c r="AY55" s="5"/>
+      <c r="AZ55" s="5"/>
     </row>
-    <row r="56" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A56" s="5" t="s">
         <v>93</v>
       </c>
@@ -6190,20 +6255,20 @@
       <c r="X56" s="5"/>
       <c r="Y56" s="5"/>
       <c r="Z56" s="5"/>
-      <c r="AA56" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB56" s="5"/>
+      <c r="AA56" s="5"/>
+      <c r="AB56" s="5">
+        <v>1</v>
+      </c>
       <c r="AC56" s="5"/>
-      <c r="AD56" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE56" s="5"/>
+      <c r="AD56" s="5"/>
+      <c r="AE56" s="5">
+        <v>1</v>
+      </c>
       <c r="AF56" s="5"/>
-      <c r="AG56" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH56" s="5"/>
+      <c r="AG56" s="5"/>
+      <c r="AH56" s="5">
+        <v>1</v>
+      </c>
       <c r="AI56" s="5"/>
       <c r="AJ56" s="5"/>
       <c r="AK56" s="5"/>
@@ -6221,8 +6286,9 @@
       <c r="AW56" s="5"/>
       <c r="AX56" s="5"/>
       <c r="AY56" s="5"/>
+      <c r="AZ56" s="5"/>
     </row>
-    <row r="57" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A57" s="11" t="s">
         <v>93</v>
       </c>
@@ -6281,20 +6347,20 @@
       <c r="X57" s="11"/>
       <c r="Y57" s="11"/>
       <c r="Z57" s="11"/>
-      <c r="AA57" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB57" s="11"/>
+      <c r="AA57" s="11"/>
+      <c r="AB57" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AC57" s="11"/>
-      <c r="AD57" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE57" s="11"/>
+      <c r="AD57" s="11"/>
+      <c r="AE57" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AF57" s="11"/>
-      <c r="AG57" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH57" s="11"/>
+      <c r="AG57" s="11"/>
+      <c r="AH57" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AI57" s="11"/>
       <c r="AJ57" s="11"/>
       <c r="AK57" s="11"/>
@@ -6312,8 +6378,9 @@
       <c r="AW57" s="11"/>
       <c r="AX57" s="11"/>
       <c r="AY57" s="11"/>
+      <c r="AZ57" s="11"/>
     </row>
-    <row r="58" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A58" s="11" t="s">
         <v>93</v>
       </c>
@@ -6372,20 +6439,20 @@
       <c r="X58" s="11"/>
       <c r="Y58" s="11"/>
       <c r="Z58" s="11"/>
-      <c r="AA58" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB58" s="11"/>
+      <c r="AA58" s="11"/>
+      <c r="AB58" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AC58" s="11"/>
-      <c r="AD58" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE58" s="11"/>
+      <c r="AD58" s="11"/>
+      <c r="AE58" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AF58" s="11"/>
-      <c r="AG58" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH58" s="11"/>
+      <c r="AG58" s="11"/>
+      <c r="AH58" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AI58" s="11"/>
       <c r="AJ58" s="11"/>
       <c r="AK58" s="11"/>
@@ -6403,8 +6470,9 @@
       <c r="AW58" s="11"/>
       <c r="AX58" s="11"/>
       <c r="AY58" s="11"/>
+      <c r="AZ58" s="11"/>
     </row>
-    <row r="59" spans="1:51" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:52" s="14" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A59" s="13" t="s">
         <v>93</v>
       </c>
@@ -6463,20 +6531,20 @@
       <c r="X59" s="13"/>
       <c r="Y59" s="13"/>
       <c r="Z59" s="13"/>
-      <c r="AA59" s="15">
-        <v>0</v>
-      </c>
-      <c r="AB59" s="13"/>
+      <c r="AA59" s="13"/>
+      <c r="AB59" s="15">
+        <v>0</v>
+      </c>
       <c r="AC59" s="13"/>
-      <c r="AD59" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE59" s="13"/>
+      <c r="AD59" s="13"/>
+      <c r="AE59" s="15">
+        <v>0</v>
+      </c>
       <c r="AF59" s="13"/>
-      <c r="AG59" s="15">
-        <v>0</v>
-      </c>
-      <c r="AH59" s="13"/>
+      <c r="AG59" s="13"/>
+      <c r="AH59" s="15">
+        <v>0</v>
+      </c>
       <c r="AI59" s="13"/>
       <c r="AJ59" s="13"/>
       <c r="AK59" s="13"/>
@@ -6494,8 +6562,9 @@
       <c r="AW59" s="13"/>
       <c r="AX59" s="13"/>
       <c r="AY59" s="13"/>
+      <c r="AZ59" s="13"/>
     </row>
-    <row r="60" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A60" s="11" t="s">
         <v>93</v>
       </c>
@@ -6554,20 +6623,20 @@
       <c r="X60" s="11"/>
       <c r="Y60" s="11"/>
       <c r="Z60" s="11"/>
-      <c r="AA60" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB60" s="11"/>
+      <c r="AA60" s="11"/>
+      <c r="AB60" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AC60" s="11"/>
-      <c r="AD60" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE60" s="11"/>
+      <c r="AD60" s="11"/>
+      <c r="AE60" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AF60" s="11"/>
-      <c r="AG60" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH60" s="11"/>
+      <c r="AG60" s="11"/>
+      <c r="AH60" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AI60" s="11"/>
       <c r="AJ60" s="11"/>
       <c r="AK60" s="11"/>
@@ -6585,8 +6654,9 @@
       <c r="AW60" s="11"/>
       <c r="AX60" s="11"/>
       <c r="AY60" s="11"/>
+      <c r="AZ60" s="11"/>
     </row>
-    <row r="61" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A61" s="9" t="s">
         <v>76</v>
       </c>
@@ -6645,20 +6715,20 @@
       <c r="X61" s="9"/>
       <c r="Y61" s="9"/>
       <c r="Z61" s="9"/>
-      <c r="AA61" s="9">
+      <c r="AA61" s="9"/>
+      <c r="AB61" s="9">
         <v>-1</v>
       </c>
-      <c r="AB61" s="9"/>
       <c r="AC61" s="9"/>
-      <c r="AD61" s="9">
+      <c r="AD61" s="9"/>
+      <c r="AE61" s="9">
         <v>-1</v>
       </c>
-      <c r="AE61" s="9"/>
       <c r="AF61" s="9"/>
-      <c r="AG61" s="9">
+      <c r="AG61" s="9"/>
+      <c r="AH61" s="9">
         <v>-1</v>
       </c>
-      <c r="AH61" s="9"/>
       <c r="AI61" s="9"/>
       <c r="AJ61" s="9"/>
       <c r="AK61" s="9"/>
@@ -6676,8 +6746,9 @@
       <c r="AW61" s="9"/>
       <c r="AX61" s="9"/>
       <c r="AY61" s="9"/>
+      <c r="AZ61" s="9"/>
     </row>
-    <row r="62" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A62" s="5" t="s">
         <v>76</v>
       </c>
@@ -6736,20 +6807,20 @@
       <c r="X62" s="5"/>
       <c r="Y62" s="5"/>
       <c r="Z62" s="5"/>
-      <c r="AA62" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB62" s="5"/>
+      <c r="AA62" s="5"/>
+      <c r="AB62" s="5">
+        <v>1</v>
+      </c>
       <c r="AC62" s="5"/>
-      <c r="AD62" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE62" s="5"/>
+      <c r="AD62" s="5"/>
+      <c r="AE62" s="5">
+        <v>1</v>
+      </c>
       <c r="AF62" s="5"/>
-      <c r="AG62" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH62" s="5"/>
+      <c r="AG62" s="5"/>
+      <c r="AH62" s="5">
+        <v>1</v>
+      </c>
       <c r="AI62" s="5"/>
       <c r="AJ62" s="5"/>
       <c r="AK62" s="5"/>
@@ -6767,8 +6838,9 @@
       <c r="AW62" s="5"/>
       <c r="AX62" s="5"/>
       <c r="AY62" s="5"/>
+      <c r="AZ62" s="5"/>
     </row>
-    <row r="63" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A63" s="11" t="s">
         <v>76</v>
       </c>
@@ -6827,20 +6899,20 @@
       <c r="X63" s="11"/>
       <c r="Y63" s="11"/>
       <c r="Z63" s="11"/>
-      <c r="AA63" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB63" s="11"/>
+      <c r="AA63" s="11"/>
+      <c r="AB63" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AC63" s="11"/>
-      <c r="AD63" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE63" s="11"/>
+      <c r="AD63" s="11"/>
+      <c r="AE63" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AF63" s="11"/>
-      <c r="AG63" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH63" s="11"/>
+      <c r="AG63" s="11"/>
+      <c r="AH63" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AI63" s="11"/>
       <c r="AJ63" s="11"/>
       <c r="AK63" s="11"/>
@@ -6858,8 +6930,9 @@
       <c r="AW63" s="11"/>
       <c r="AX63" s="11"/>
       <c r="AY63" s="11"/>
+      <c r="AZ63" s="11"/>
     </row>
-    <row r="64" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A64" s="5" t="s">
         <v>76</v>
       </c>
@@ -6918,20 +6991,20 @@
       <c r="X64" s="5"/>
       <c r="Y64" s="5"/>
       <c r="Z64" s="5"/>
-      <c r="AA64" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB64" s="5"/>
+      <c r="AA64" s="5"/>
+      <c r="AB64" s="5">
+        <v>1</v>
+      </c>
       <c r="AC64" s="5"/>
-      <c r="AD64" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE64" s="5"/>
+      <c r="AD64" s="5"/>
+      <c r="AE64" s="5">
+        <v>1</v>
+      </c>
       <c r="AF64" s="5"/>
-      <c r="AG64" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH64" s="5"/>
+      <c r="AG64" s="5"/>
+      <c r="AH64" s="5">
+        <v>1</v>
+      </c>
       <c r="AI64" s="5"/>
       <c r="AJ64" s="5"/>
       <c r="AK64" s="5"/>
@@ -6949,8 +7022,9 @@
       <c r="AW64" s="5"/>
       <c r="AX64" s="5"/>
       <c r="AY64" s="5"/>
+      <c r="AZ64" s="5"/>
     </row>
-    <row r="65" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A65" s="11" t="s">
         <v>76</v>
       </c>
@@ -7009,20 +7083,20 @@
       <c r="X65" s="11"/>
       <c r="Y65" s="11"/>
       <c r="Z65" s="11"/>
-      <c r="AA65" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB65" s="11"/>
+      <c r="AA65" s="11"/>
+      <c r="AB65" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AC65" s="11"/>
-      <c r="AD65" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE65" s="11"/>
+      <c r="AD65" s="11"/>
+      <c r="AE65" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AF65" s="11"/>
-      <c r="AG65" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH65" s="11"/>
+      <c r="AG65" s="11"/>
+      <c r="AH65" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AI65" s="11"/>
       <c r="AJ65" s="11"/>
       <c r="AK65" s="11"/>
@@ -7040,8 +7114,9 @@
       <c r="AW65" s="11"/>
       <c r="AX65" s="11"/>
       <c r="AY65" s="11"/>
+      <c r="AZ65" s="11"/>
     </row>
-    <row r="66" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A66" s="5" t="s">
         <v>76</v>
       </c>
@@ -7100,20 +7175,20 @@
       <c r="X66" s="5"/>
       <c r="Y66" s="5"/>
       <c r="Z66" s="5"/>
-      <c r="AA66" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB66" s="5"/>
+      <c r="AA66" s="5"/>
+      <c r="AB66" s="5">
+        <v>1</v>
+      </c>
       <c r="AC66" s="5"/>
-      <c r="AD66" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE66" s="5"/>
+      <c r="AD66" s="5"/>
+      <c r="AE66" s="5">
+        <v>1</v>
+      </c>
       <c r="AF66" s="5"/>
-      <c r="AG66" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH66" s="5"/>
+      <c r="AG66" s="5"/>
+      <c r="AH66" s="5">
+        <v>1</v>
+      </c>
       <c r="AI66" s="5"/>
       <c r="AJ66" s="5"/>
       <c r="AK66" s="5"/>
@@ -7131,8 +7206,9 @@
       <c r="AW66" s="5"/>
       <c r="AX66" s="5"/>
       <c r="AY66" s="5"/>
+      <c r="AZ66" s="5"/>
     </row>
-    <row r="67" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A67" s="5" t="s">
         <v>76</v>
       </c>
@@ -7191,20 +7267,20 @@
       <c r="X67" s="5"/>
       <c r="Y67" s="5"/>
       <c r="Z67" s="5"/>
-      <c r="AA67" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB67" s="5"/>
+      <c r="AA67" s="5"/>
+      <c r="AB67" s="5">
+        <v>1</v>
+      </c>
       <c r="AC67" s="5"/>
-      <c r="AD67" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE67" s="5"/>
+      <c r="AD67" s="5"/>
+      <c r="AE67" s="5">
+        <v>1</v>
+      </c>
       <c r="AF67" s="5"/>
-      <c r="AG67" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH67" s="5"/>
+      <c r="AG67" s="5"/>
+      <c r="AH67" s="5">
+        <v>1</v>
+      </c>
       <c r="AI67" s="5"/>
       <c r="AJ67" s="5"/>
       <c r="AK67" s="5"/>
@@ -7222,8 +7298,9 @@
       <c r="AW67" s="5"/>
       <c r="AX67" s="5"/>
       <c r="AY67" s="5"/>
+      <c r="AZ67" s="5"/>
     </row>
-    <row r="68" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A68" s="5" t="s">
         <v>76</v>
       </c>
@@ -7282,20 +7359,20 @@
       <c r="X68" s="5"/>
       <c r="Y68" s="5"/>
       <c r="Z68" s="5"/>
-      <c r="AA68" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB68" s="5"/>
+      <c r="AA68" s="5"/>
+      <c r="AB68" s="5">
+        <v>1</v>
+      </c>
       <c r="AC68" s="5"/>
-      <c r="AD68" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE68" s="5"/>
+      <c r="AD68" s="5"/>
+      <c r="AE68" s="5">
+        <v>1</v>
+      </c>
       <c r="AF68" s="5"/>
-      <c r="AG68" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH68" s="5"/>
+      <c r="AG68" s="5"/>
+      <c r="AH68" s="5">
+        <v>1</v>
+      </c>
       <c r="AI68" s="5"/>
       <c r="AJ68" s="5"/>
       <c r="AK68" s="5"/>
@@ -7313,8 +7390,9 @@
       <c r="AW68" s="5"/>
       <c r="AX68" s="5"/>
       <c r="AY68" s="5"/>
+      <c r="AZ68" s="5"/>
     </row>
-    <row r="69" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A69" s="5" t="s">
         <v>76</v>
       </c>
@@ -7373,20 +7451,20 @@
       <c r="X69" s="5"/>
       <c r="Y69" s="5"/>
       <c r="Z69" s="5"/>
-      <c r="AA69" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB69" s="5"/>
+      <c r="AA69" s="5"/>
+      <c r="AB69" s="8">
+        <v>0</v>
+      </c>
       <c r="AC69" s="5"/>
-      <c r="AD69" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE69" s="5"/>
+      <c r="AD69" s="5"/>
+      <c r="AE69" s="8">
+        <v>0</v>
+      </c>
       <c r="AF69" s="5"/>
-      <c r="AG69" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH69" s="5"/>
+      <c r="AG69" s="5"/>
+      <c r="AH69" s="8">
+        <v>0</v>
+      </c>
       <c r="AI69" s="5"/>
       <c r="AJ69" s="5"/>
       <c r="AK69" s="5"/>
@@ -7404,8 +7482,9 @@
       <c r="AW69" s="5"/>
       <c r="AX69" s="5"/>
       <c r="AY69" s="5"/>
+      <c r="AZ69" s="5"/>
     </row>
-    <row r="70" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A70" s="5" t="s">
         <v>76</v>
       </c>
@@ -7464,20 +7543,20 @@
       <c r="X70" s="5"/>
       <c r="Y70" s="5"/>
       <c r="Z70" s="5"/>
-      <c r="AA70" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB70" s="5"/>
+      <c r="AA70" s="5"/>
+      <c r="AB70" s="5">
+        <v>1</v>
+      </c>
       <c r="AC70" s="5"/>
-      <c r="AD70" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE70" s="5"/>
+      <c r="AD70" s="5"/>
+      <c r="AE70" s="5">
+        <v>1</v>
+      </c>
       <c r="AF70" s="5"/>
-      <c r="AG70" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH70" s="5"/>
+      <c r="AG70" s="5"/>
+      <c r="AH70" s="5">
+        <v>1</v>
+      </c>
       <c r="AI70" s="5"/>
       <c r="AJ70" s="5"/>
       <c r="AK70" s="5"/>
@@ -7495,8 +7574,9 @@
       <c r="AW70" s="5"/>
       <c r="AX70" s="5"/>
       <c r="AY70" s="5"/>
+      <c r="AZ70" s="5"/>
     </row>
-    <row r="71" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A71" s="5" t="s">
         <v>76</v>
       </c>
@@ -7555,20 +7635,20 @@
       <c r="X71" s="5"/>
       <c r="Y71" s="5"/>
       <c r="Z71" s="5"/>
-      <c r="AA71" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB71" s="5"/>
+      <c r="AA71" s="5"/>
+      <c r="AB71" s="5">
+        <v>1</v>
+      </c>
       <c r="AC71" s="5"/>
-      <c r="AD71" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE71" s="5"/>
+      <c r="AD71" s="5"/>
+      <c r="AE71" s="5">
+        <v>1</v>
+      </c>
       <c r="AF71" s="5"/>
-      <c r="AG71" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH71" s="5"/>
+      <c r="AG71" s="5"/>
+      <c r="AH71" s="5">
+        <v>1</v>
+      </c>
       <c r="AI71" s="5"/>
       <c r="AJ71" s="5"/>
       <c r="AK71" s="5"/>
@@ -7586,8 +7666,9 @@
       <c r="AW71" s="5"/>
       <c r="AX71" s="5"/>
       <c r="AY71" s="5"/>
+      <c r="AZ71" s="5"/>
     </row>
-    <row r="72" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A72" s="5" t="s">
         <v>76</v>
       </c>
@@ -7646,20 +7727,20 @@
       <c r="X72" s="5"/>
       <c r="Y72" s="5"/>
       <c r="Z72" s="5"/>
-      <c r="AA72" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB72" s="5"/>
+      <c r="AA72" s="5"/>
+      <c r="AB72" s="5">
+        <v>1</v>
+      </c>
       <c r="AC72" s="5"/>
-      <c r="AD72" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE72" s="5"/>
+      <c r="AD72" s="5"/>
+      <c r="AE72" s="5">
+        <v>1</v>
+      </c>
       <c r="AF72" s="5"/>
-      <c r="AG72" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH72" s="5"/>
+      <c r="AG72" s="5"/>
+      <c r="AH72" s="5">
+        <v>1</v>
+      </c>
       <c r="AI72" s="5"/>
       <c r="AJ72" s="5"/>
       <c r="AK72" s="5"/>
@@ -7677,8 +7758,9 @@
       <c r="AW72" s="5"/>
       <c r="AX72" s="5"/>
       <c r="AY72" s="5"/>
+      <c r="AZ72" s="5"/>
     </row>
-    <row r="73" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A73" s="5" t="s">
         <v>76</v>
       </c>
@@ -7737,20 +7819,20 @@
       <c r="X73" s="5"/>
       <c r="Y73" s="5"/>
       <c r="Z73" s="5"/>
-      <c r="AA73" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB73" s="5"/>
+      <c r="AA73" s="5"/>
+      <c r="AB73" s="5">
+        <v>1</v>
+      </c>
       <c r="AC73" s="5"/>
-      <c r="AD73" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE73" s="5"/>
+      <c r="AD73" s="5"/>
+      <c r="AE73" s="5">
+        <v>1</v>
+      </c>
       <c r="AF73" s="5"/>
-      <c r="AG73" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH73" s="5"/>
+      <c r="AG73" s="5"/>
+      <c r="AH73" s="5">
+        <v>1</v>
+      </c>
       <c r="AI73" s="5"/>
       <c r="AJ73" s="5"/>
       <c r="AK73" s="5"/>
@@ -7768,8 +7850,9 @@
       <c r="AW73" s="5"/>
       <c r="AX73" s="5"/>
       <c r="AY73" s="5"/>
+      <c r="AZ73" s="5"/>
     </row>
-    <row r="74" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A74" s="11" t="s">
         <v>76</v>
       </c>
@@ -7828,20 +7911,20 @@
       <c r="X74" s="11"/>
       <c r="Y74" s="11"/>
       <c r="Z74" s="11"/>
-      <c r="AA74" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB74" s="11"/>
+      <c r="AA74" s="11"/>
+      <c r="AB74" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AC74" s="11"/>
-      <c r="AD74" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE74" s="11"/>
+      <c r="AD74" s="11"/>
+      <c r="AE74" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AF74" s="11"/>
-      <c r="AG74" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH74" s="11"/>
+      <c r="AG74" s="11"/>
+      <c r="AH74" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AI74" s="11"/>
       <c r="AJ74" s="11"/>
       <c r="AK74" s="11"/>
@@ -7859,8 +7942,9 @@
       <c r="AW74" s="11"/>
       <c r="AX74" s="11"/>
       <c r="AY74" s="11"/>
+      <c r="AZ74" s="11"/>
     </row>
-    <row r="75" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A75" s="5" t="s">
         <v>76</v>
       </c>
@@ -7919,20 +8003,20 @@
       <c r="X75" s="5"/>
       <c r="Y75" s="5"/>
       <c r="Z75" s="5"/>
-      <c r="AA75" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB75" s="5"/>
+      <c r="AA75" s="5"/>
+      <c r="AB75" s="8">
+        <v>0</v>
+      </c>
       <c r="AC75" s="5"/>
-      <c r="AD75" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE75" s="5"/>
+      <c r="AD75" s="5"/>
+      <c r="AE75" s="8">
+        <v>0</v>
+      </c>
       <c r="AF75" s="5"/>
-      <c r="AG75" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH75" s="5"/>
+      <c r="AG75" s="5"/>
+      <c r="AH75" s="8">
+        <v>0</v>
+      </c>
       <c r="AI75" s="5"/>
       <c r="AJ75" s="5"/>
       <c r="AK75" s="5"/>
@@ -7950,8 +8034,9 @@
       <c r="AW75" s="5"/>
       <c r="AX75" s="5"/>
       <c r="AY75" s="5"/>
+      <c r="AZ75" s="5"/>
     </row>
-    <row r="76" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A76" s="5" t="s">
         <v>76</v>
       </c>
@@ -8010,20 +8095,20 @@
       <c r="X76" s="5"/>
       <c r="Y76" s="5"/>
       <c r="Z76" s="5"/>
-      <c r="AA76" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB76" s="5"/>
+      <c r="AA76" s="5"/>
+      <c r="AB76" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC76" s="5"/>
-      <c r="AD76" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE76" s="5"/>
+      <c r="AD76" s="5"/>
+      <c r="AE76" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF76" s="5"/>
-      <c r="AG76" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH76" s="5"/>
+      <c r="AG76" s="5"/>
+      <c r="AH76" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI76" s="5"/>
       <c r="AJ76" s="5"/>
       <c r="AK76" s="5"/>
@@ -8041,8 +8126,9 @@
       <c r="AW76" s="5"/>
       <c r="AX76" s="5"/>
       <c r="AY76" s="5"/>
+      <c r="AZ76" s="5"/>
     </row>
-    <row r="77" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A77" s="5" t="s">
         <v>76</v>
       </c>
@@ -8101,20 +8187,20 @@
       <c r="X77" s="5"/>
       <c r="Y77" s="5"/>
       <c r="Z77" s="5"/>
-      <c r="AA77" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB77" s="5"/>
+      <c r="AA77" s="5"/>
+      <c r="AB77" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC77" s="5"/>
-      <c r="AD77" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE77" s="5"/>
+      <c r="AD77" s="5"/>
+      <c r="AE77" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF77" s="5"/>
-      <c r="AG77" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH77" s="5"/>
+      <c r="AG77" s="5"/>
+      <c r="AH77" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI77" s="5"/>
       <c r="AJ77" s="5"/>
       <c r="AK77" s="5"/>
@@ -8132,8 +8218,9 @@
       <c r="AW77" s="5"/>
       <c r="AX77" s="5"/>
       <c r="AY77" s="5"/>
+      <c r="AZ77" s="5"/>
     </row>
-    <row r="78" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A78" s="5" t="s">
         <v>76</v>
       </c>
@@ -8192,20 +8279,20 @@
       <c r="X78" s="5"/>
       <c r="Y78" s="5"/>
       <c r="Z78" s="5"/>
-      <c r="AA78" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB78" s="5"/>
+      <c r="AA78" s="5"/>
+      <c r="AB78" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC78" s="5"/>
-      <c r="AD78" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE78" s="5"/>
+      <c r="AD78" s="5"/>
+      <c r="AE78" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF78" s="5"/>
-      <c r="AG78" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH78" s="5"/>
+      <c r="AG78" s="5"/>
+      <c r="AH78" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI78" s="5"/>
       <c r="AJ78" s="5"/>
       <c r="AK78" s="5"/>
@@ -8223,8 +8310,9 @@
       <c r="AW78" s="5"/>
       <c r="AX78" s="5"/>
       <c r="AY78" s="5"/>
+      <c r="AZ78" s="5"/>
     </row>
-    <row r="79" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A79" s="5" t="s">
         <v>76</v>
       </c>
@@ -8283,20 +8371,20 @@
       <c r="X79" s="5"/>
       <c r="Y79" s="5"/>
       <c r="Z79" s="5"/>
-      <c r="AA79" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB79" s="5"/>
+      <c r="AA79" s="5"/>
+      <c r="AB79" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC79" s="5"/>
-      <c r="AD79" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE79" s="5"/>
+      <c r="AD79" s="5"/>
+      <c r="AE79" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF79" s="5"/>
-      <c r="AG79" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH79" s="5"/>
+      <c r="AG79" s="5"/>
+      <c r="AH79" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI79" s="5"/>
       <c r="AJ79" s="5"/>
       <c r="AK79" s="5"/>
@@ -8314,8 +8402,9 @@
       <c r="AW79" s="5"/>
       <c r="AX79" s="5"/>
       <c r="AY79" s="5"/>
+      <c r="AZ79" s="5"/>
     </row>
-    <row r="80" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A80" s="5" t="s">
         <v>76</v>
       </c>
@@ -8374,20 +8463,20 @@
       <c r="X80" s="5"/>
       <c r="Y80" s="5"/>
       <c r="Z80" s="5"/>
-      <c r="AA80" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB80" s="5"/>
+      <c r="AA80" s="5"/>
+      <c r="AB80" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC80" s="5"/>
-      <c r="AD80" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE80" s="5"/>
+      <c r="AD80" s="5"/>
+      <c r="AE80" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF80" s="5"/>
-      <c r="AG80" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH80" s="5"/>
+      <c r="AG80" s="5"/>
+      <c r="AH80" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI80" s="5"/>
       <c r="AJ80" s="5"/>
       <c r="AK80" s="5"/>
@@ -8405,8 +8494,9 @@
       <c r="AW80" s="5"/>
       <c r="AX80" s="5"/>
       <c r="AY80" s="5"/>
+      <c r="AZ80" s="5"/>
     </row>
-    <row r="81" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A81" s="5" t="s">
         <v>76</v>
       </c>
@@ -8465,20 +8555,20 @@
       <c r="X81" s="5"/>
       <c r="Y81" s="5"/>
       <c r="Z81" s="5"/>
-      <c r="AA81" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB81" s="5"/>
+      <c r="AA81" s="5"/>
+      <c r="AB81" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC81" s="5"/>
-      <c r="AD81" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE81" s="5"/>
+      <c r="AD81" s="5"/>
+      <c r="AE81" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF81" s="5"/>
-      <c r="AG81" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH81" s="5"/>
+      <c r="AG81" s="5"/>
+      <c r="AH81" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI81" s="5"/>
       <c r="AJ81" s="5"/>
       <c r="AK81" s="5"/>
@@ -8496,8 +8586,9 @@
       <c r="AW81" s="5"/>
       <c r="AX81" s="5"/>
       <c r="AY81" s="5"/>
+      <c r="AZ81" s="5"/>
     </row>
-    <row r="82" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A82" s="5" t="s">
         <v>76</v>
       </c>
@@ -8556,20 +8647,20 @@
       <c r="X82" s="5"/>
       <c r="Y82" s="5"/>
       <c r="Z82" s="5"/>
-      <c r="AA82" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB82" s="5"/>
+      <c r="AA82" s="5"/>
+      <c r="AB82" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC82" s="5"/>
-      <c r="AD82" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE82" s="5"/>
+      <c r="AD82" s="5"/>
+      <c r="AE82" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF82" s="5"/>
-      <c r="AG82" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH82" s="5"/>
+      <c r="AG82" s="5"/>
+      <c r="AH82" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI82" s="5"/>
       <c r="AJ82" s="5"/>
       <c r="AK82" s="5"/>
@@ -8587,8 +8678,9 @@
       <c r="AW82" s="5"/>
       <c r="AX82" s="5"/>
       <c r="AY82" s="5"/>
+      <c r="AZ82" s="5"/>
     </row>
-    <row r="83" spans="1:51" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A83" s="11" t="s">
         <v>76</v>
       </c>
@@ -8647,20 +8739,20 @@
       <c r="X83" s="11"/>
       <c r="Y83" s="11"/>
       <c r="Z83" s="11"/>
-      <c r="AA83" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB83" s="11"/>
+      <c r="AA83" s="11"/>
+      <c r="AB83" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AC83" s="11"/>
-      <c r="AD83" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE83" s="11"/>
+      <c r="AD83" s="11"/>
+      <c r="AE83" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AF83" s="11"/>
-      <c r="AG83" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH83" s="11"/>
+      <c r="AG83" s="11"/>
+      <c r="AH83" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AI83" s="11"/>
       <c r="AJ83" s="11"/>
       <c r="AK83" s="11"/>
@@ -8678,8 +8770,9 @@
       <c r="AW83" s="11"/>
       <c r="AX83" s="11"/>
       <c r="AY83" s="11"/>
+      <c r="AZ83" s="11"/>
     </row>
-    <row r="84" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A84" s="5" t="s">
         <v>76</v>
       </c>
@@ -8738,20 +8831,20 @@
       <c r="X84" s="5"/>
       <c r="Y84" s="5"/>
       <c r="Z84" s="5"/>
-      <c r="AA84" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB84" s="5"/>
+      <c r="AA84" s="5"/>
+      <c r="AB84" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC84" s="5"/>
-      <c r="AD84" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE84" s="5"/>
+      <c r="AD84" s="5"/>
+      <c r="AE84" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AF84" s="5"/>
-      <c r="AG84" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH84" s="5"/>
+      <c r="AG84" s="5"/>
+      <c r="AH84" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AI84" s="5"/>
       <c r="AJ84" s="5"/>
       <c r="AK84" s="5"/>
@@ -8769,8 +8862,9 @@
       <c r="AW84" s="5"/>
       <c r="AX84" s="5"/>
       <c r="AY84" s="5"/>
+      <c r="AZ84" s="5"/>
     </row>
-    <row r="85" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A85" s="5" t="s">
         <v>76</v>
       </c>
@@ -8828,22 +8922,22 @@
       <c r="W85" s="5"/>
       <c r="X85" s="5"/>
       <c r="Y85" s="5"/>
-      <c r="Z85" s="16"/>
-      <c r="AA85" s="16">
-        <v>1</v>
-      </c>
-      <c r="AB85" s="16"/>
+      <c r="Z85" s="5"/>
+      <c r="AA85" s="16"/>
+      <c r="AB85" s="16">
+        <v>1</v>
+      </c>
       <c r="AC85" s="16"/>
-      <c r="AD85" s="16">
-        <v>1</v>
-      </c>
-      <c r="AE85" s="16"/>
+      <c r="AD85" s="16"/>
+      <c r="AE85" s="16">
+        <v>1</v>
+      </c>
       <c r="AF85" s="16"/>
-      <c r="AG85" s="16">
-        <v>1</v>
-      </c>
-      <c r="AH85" s="16"/>
-      <c r="AI85" s="5"/>
+      <c r="AG85" s="16"/>
+      <c r="AH85" s="16">
+        <v>1</v>
+      </c>
+      <c r="AI85" s="16"/>
       <c r="AJ85" s="5"/>
       <c r="AK85" s="5"/>
       <c r="AL85" s="5"/>
@@ -8860,26 +8954,27 @@
       <c r="AW85" s="5"/>
       <c r="AX85" s="5"/>
       <c r="AY85" s="5"/>
+      <c r="AZ85" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="Z1:AI1"/>
+    <mergeCell ref="AK1:AZ1"/>
+    <mergeCell ref="T2:W2"/>
+    <mergeCell ref="AA2:AC2"/>
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AP2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="J1:X1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:R2"/>
-    <mergeCell ref="AU2:AV2"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="J1:W1"/>
-    <mergeCell ref="Y1:AH1"/>
-    <mergeCell ref="AJ1:AY1"/>
-    <mergeCell ref="T2:W2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AO2:AR2"/>
-    <mergeCell ref="AS2:AT2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
MAJOR UPDATE on ECG epoching
</commit_message>
<xml_diff>
--- a/meta/MEG_ANALYSIS_MASTERFILE.xlsx
+++ b/meta/MEG_ANALYSIS_MASTERFILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\meditation\ERC\Analyses\MEG\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536EC4EB-B849-4628-A431-D6B31DCBD3E0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782C9F0B-C79B-456E-9D96-2F3D088A89F8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="180">
   <si>
     <t>ANATOMY</t>
   </si>
@@ -533,6 +533,39 @@
   </si>
   <si>
     <t>bad</t>
+  </si>
+  <si>
+    <t>MLT41|MLT43|MLT44|MLT51|MLT53|MLT54|MLT55</t>
+  </si>
+  <si>
+    <t>MLT22|MLT31|MLT32|MLT33|MLT41|MLT42|MLT43|MLT51|MLT52|MLT53|MLT54|MRF11|MRF12|MRF13|MRF14|MRF24|MRF25|MRT11|MRT21|MRT22|MRT23|MRT31|MRT32|MRT33|MRT34|MRT41|MRT42|MRT43|MRT44|MRT51|MRT52|MRT53|MRT54|MRT55</t>
+  </si>
+  <si>
+    <t>MLF14|MLT31|MLT32|MLT33|MLT34|MLT35|MLT41|MLT42|MLT43|MLT44|MLT45|MLT51|MLT52|MLT53|MLT54|MLT55|MLT56|MRF14|MRT21|MRT31|MRT32|MRT33|MRT41|MRT42|MRT43|MRT51|MRT52</t>
+  </si>
+  <si>
+    <t>MLT31|MLT41|MLT42|MLT51|MLT52|MRT31|MRT32|MRT33|MRT34|MRT41|MRT42|MRT43|MRT44|MRT51|MRT52|MRT53|MRT54|MRT55|MRT56|MRT57</t>
+  </si>
+  <si>
+    <t>MRT21|MRT22|MRT31|MRT32|MRT41|MRT42|MRT51|MRT52</t>
+  </si>
+  <si>
+    <t>MRT51|MRT52|MRT53</t>
+  </si>
+  <si>
+    <t>MLT51|MLT52</t>
+  </si>
+  <si>
+    <t>MRT52|MRT53</t>
+  </si>
+  <si>
+    <t>MRT41|MRT51|MRT52</t>
+  </si>
+  <si>
+    <t>MLF11|MLF12|MLF13|MLF14|MLT21|MLT31|MLT32|MLT41|MLT42|MLT51|MLT52</t>
+  </si>
+  <si>
+    <t>MLT41|MLT42|MLT43|MLT44|MLT51|MLT52|MLT53|MLT54</t>
   </si>
 </sst>
 </file>
@@ -657,7 +690,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -700,6 +733,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1107,81 +1155,85 @@
   <dimension ref="A1:AZ85"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="O30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="X5" sqref="X5"/>
+      <selection pane="bottomRight" activeCell="X41" sqref="X41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="21" max="21" width="9.06640625" style="21"/>
+    <col min="24" max="24" width="9.06640625" style="21"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="C1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
+      <c r="J1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
       <c r="Y1" s="1"/>
-      <c r="Z1" s="21" t="s">
+      <c r="Z1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21"/>
-      <c r="AI1" s="21"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
       <c r="AJ1" s="1"/>
-      <c r="AK1" s="21" t="s">
+      <c r="AK1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="21"/>
-      <c r="AM1" s="21"/>
-      <c r="AN1" s="21"/>
-      <c r="AO1" s="21"/>
-      <c r="AP1" s="21"/>
-      <c r="AQ1" s="21"/>
-      <c r="AR1" s="21"/>
-      <c r="AS1" s="21"/>
-      <c r="AT1" s="21"/>
-      <c r="AU1" s="21"/>
-      <c r="AV1" s="21"/>
-      <c r="AW1" s="21"/>
-      <c r="AX1" s="21"/>
-      <c r="AY1" s="21"/>
-      <c r="AZ1" s="21"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="26"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="26"/>
+      <c r="AZ1" s="26"/>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.45">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1189,32 +1241,32 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="19" t="s">
+      <c r="K2" s="23"/>
+      <c r="L2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19" t="s">
+      <c r="M2" s="24"/>
+      <c r="N2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19" t="s">
+      <c r="O2" s="24"/>
+      <c r="P2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
       <c r="S2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="22" t="s">
+      <c r="T2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
       <c r="X2" s="3" t="s">
         <v>167</v>
       </c>
@@ -1222,21 +1274,21 @@
       <c r="Z2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="23" t="s">
+      <c r="AA2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="23"/>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="23" t="s">
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="AE2" s="23"/>
-      <c r="AF2" s="23"/>
-      <c r="AG2" s="23" t="s">
+      <c r="AE2" s="28"/>
+      <c r="AF2" s="28"/>
+      <c r="AG2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AH2" s="23"/>
-      <c r="AI2" s="23"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="28"/>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1" t="s">
         <v>15</v>
@@ -1244,27 +1296,27 @@
       <c r="AL2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AM2" s="17" t="s">
+      <c r="AM2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="AN2" s="17"/>
+      <c r="AN2" s="22"/>
       <c r="AO2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AP2" s="17" t="s">
+      <c r="AP2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="AQ2" s="17"/>
-      <c r="AR2" s="17"/>
-      <c r="AS2" s="17"/>
-      <c r="AT2" s="17" t="s">
+      <c r="AQ2" s="22"/>
+      <c r="AR2" s="22"/>
+      <c r="AS2" s="22"/>
+      <c r="AT2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="AU2" s="17"/>
-      <c r="AV2" s="17" t="s">
+      <c r="AU2" s="22"/>
+      <c r="AV2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="AW2" s="17"/>
+      <c r="AW2" s="22"/>
       <c r="AX2" s="1"/>
       <c r="AY2" s="1"/>
       <c r="AZ2" s="1"/>
@@ -1556,12 +1608,12 @@
       <c r="T5" s="5">
         <v>1</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="U5" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
+      <c r="X5" s="17"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
@@ -1648,12 +1700,12 @@
       <c r="T6" s="9">
         <v>1</v>
       </c>
-      <c r="U6" s="9" t="s">
+      <c r="U6" s="18" t="s">
         <v>78</v>
       </c>
       <c r="V6" s="9"/>
       <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
+      <c r="X6" s="18"/>
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
       <c r="AA6" s="9"/>
@@ -1740,12 +1792,12 @@
       <c r="T7" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U7" s="5" t="s">
+      <c r="U7" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
+      <c r="X7" s="17"/>
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
@@ -1832,12 +1884,12 @@
       <c r="T8" s="5">
         <v>1</v>
       </c>
-      <c r="U8" s="5" t="s">
+      <c r="U8" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
+      <c r="X8" s="17"/>
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
@@ -1924,12 +1976,12 @@
       <c r="T9" s="9">
         <v>1</v>
       </c>
-      <c r="U9" s="9" t="s">
+      <c r="U9" s="18" t="s">
         <v>78</v>
       </c>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
-      <c r="X9" s="9"/>
+      <c r="X9" s="18"/>
       <c r="Y9" s="9"/>
       <c r="Z9" s="9"/>
       <c r="AA9" s="9"/>
@@ -2016,12 +2068,12 @@
       <c r="T10" s="9">
         <v>1</v>
       </c>
-      <c r="U10" s="9" t="s">
+      <c r="U10" s="18" t="s">
         <v>78</v>
       </c>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
+      <c r="X10" s="18"/>
       <c r="Y10" s="9"/>
       <c r="Z10" s="9"/>
       <c r="AA10" s="9"/>
@@ -2108,12 +2160,12 @@
       <c r="T11" s="5">
         <v>1</v>
       </c>
-      <c r="U11" s="5" t="s">
+      <c r="U11" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
+      <c r="X11" s="17"/>
       <c r="Y11" s="5"/>
       <c r="Z11" s="5"/>
       <c r="AA11" s="5"/>
@@ -2200,12 +2252,12 @@
       <c r="T12" s="5">
         <v>1</v>
       </c>
-      <c r="U12" s="5" t="s">
+      <c r="U12" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
+      <c r="X12" s="17"/>
       <c r="Y12" s="5"/>
       <c r="Z12" s="5"/>
       <c r="AA12" s="5"/>
@@ -2292,12 +2344,14 @@
       <c r="T13" s="5">
         <v>1</v>
       </c>
-      <c r="U13" s="5" t="s">
+      <c r="U13" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
+      <c r="X13" s="17" t="s">
+        <v>169</v>
+      </c>
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
       <c r="AA13" s="5"/>
@@ -2384,12 +2438,12 @@
       <c r="T14" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U14" s="5" t="s">
+      <c r="U14" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
+      <c r="X14" s="17"/>
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
       <c r="AA14" s="5"/>
@@ -2476,12 +2530,12 @@
       <c r="T15" s="5">
         <v>1</v>
       </c>
-      <c r="U15" s="5" t="s">
+      <c r="U15" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V15" s="5"/>
       <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
+      <c r="X15" s="17"/>
       <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
       <c r="AA15" s="5"/>
@@ -2568,12 +2622,12 @@
       <c r="T16" s="11">
         <v>1</v>
       </c>
-      <c r="U16" s="11" t="s">
+      <c r="U16" s="19" t="s">
         <v>78</v>
       </c>
       <c r="V16" s="11"/>
       <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
+      <c r="X16" s="19"/>
       <c r="Y16" s="11"/>
       <c r="Z16" s="11"/>
       <c r="AA16" s="11"/>
@@ -2660,12 +2714,12 @@
       <c r="T17" s="11">
         <v>1</v>
       </c>
-      <c r="U17" s="11" t="s">
+      <c r="U17" s="19" t="s">
         <v>78</v>
       </c>
       <c r="V17" s="11"/>
       <c r="W17" s="11"/>
-      <c r="X17" s="11"/>
+      <c r="X17" s="19"/>
       <c r="Y17" s="11"/>
       <c r="Z17" s="11"/>
       <c r="AA17" s="11"/>
@@ -2752,12 +2806,12 @@
       <c r="T18" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="U18" s="11" t="s">
+      <c r="U18" s="19" t="s">
         <v>90</v>
       </c>
       <c r="V18" s="11"/>
       <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
+      <c r="X18" s="19"/>
       <c r="Y18" s="11"/>
       <c r="Z18" s="11"/>
       <c r="AA18" s="11"/>
@@ -2844,12 +2898,12 @@
       <c r="T19" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="U19" s="11" t="s">
+      <c r="U19" s="19" t="s">
         <v>90</v>
       </c>
       <c r="V19" s="11"/>
       <c r="W19" s="11"/>
-      <c r="X19" s="11"/>
+      <c r="X19" s="19"/>
       <c r="Y19" s="11"/>
       <c r="Z19" s="11"/>
       <c r="AA19" s="11"/>
@@ -2936,12 +2990,12 @@
       <c r="T20" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="U20" s="11" t="s">
+      <c r="U20" s="19" t="s">
         <v>90</v>
       </c>
       <c r="V20" s="11"/>
       <c r="W20" s="11"/>
-      <c r="X20" s="11"/>
+      <c r="X20" s="19"/>
       <c r="Y20" s="11"/>
       <c r="Z20" s="11"/>
       <c r="AA20" s="11"/>
@@ -3028,12 +3082,12 @@
       <c r="T21" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="U21" s="11" t="s">
+      <c r="U21" s="19" t="s">
         <v>90</v>
       </c>
       <c r="V21" s="11"/>
       <c r="W21" s="11"/>
-      <c r="X21" s="11"/>
+      <c r="X21" s="19"/>
       <c r="Y21" s="11"/>
       <c r="Z21" s="11"/>
       <c r="AA21" s="11"/>
@@ -3120,12 +3174,12 @@
       <c r="T22" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U22" s="5" t="s">
+      <c r="U22" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V22" s="5"/>
       <c r="W22" s="5"/>
-      <c r="X22" s="5"/>
+      <c r="X22" s="17"/>
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
       <c r="AA22" s="5"/>
@@ -3212,12 +3266,12 @@
       <c r="T23" s="5">
         <v>1</v>
       </c>
-      <c r="U23" s="5" t="s">
+      <c r="U23" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V23" s="5"/>
       <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
+      <c r="X23" s="17"/>
       <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
       <c r="AA23" s="5"/>
@@ -3304,12 +3358,12 @@
       <c r="T24" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U24" s="5" t="s">
+      <c r="U24" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V24" s="5"/>
       <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
+      <c r="X24" s="17"/>
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
@@ -3396,12 +3450,14 @@
       <c r="T25" s="5">
         <v>1</v>
       </c>
-      <c r="U25" s="5" t="s">
+      <c r="U25" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V25" s="5"/>
       <c r="W25" s="5"/>
-      <c r="X25" s="5"/>
+      <c r="X25" s="17" t="s">
+        <v>170</v>
+      </c>
       <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
       <c r="AA25" s="5"/>
@@ -3488,12 +3544,12 @@
       <c r="T26" s="5">
         <v>1</v>
       </c>
-      <c r="U26" s="5" t="s">
+      <c r="U26" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V26" s="5"/>
       <c r="W26" s="5"/>
-      <c r="X26" s="5"/>
+      <c r="X26" s="17"/>
       <c r="Y26" s="5"/>
       <c r="Z26" s="5"/>
       <c r="AA26" s="5"/>
@@ -3580,12 +3636,12 @@
       <c r="T27" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U27" s="5" t="s">
+      <c r="U27" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V27" s="5"/>
       <c r="W27" s="5"/>
-      <c r="X27" s="5"/>
+      <c r="X27" s="17"/>
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
       <c r="AA27" s="5"/>
@@ -3672,12 +3728,12 @@
       <c r="T28" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U28" s="5" t="s">
+      <c r="U28" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V28" s="5"/>
       <c r="W28" s="5"/>
-      <c r="X28" s="5"/>
+      <c r="X28" s="17"/>
       <c r="Y28" s="5"/>
       <c r="Z28" s="5"/>
       <c r="AA28" s="5"/>
@@ -3764,12 +3820,12 @@
       <c r="T29" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U29" s="5" t="s">
+      <c r="U29" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V29" s="5"/>
       <c r="W29" s="5"/>
-      <c r="X29" s="5"/>
+      <c r="X29" s="17"/>
       <c r="Y29" s="5"/>
       <c r="Z29" s="5"/>
       <c r="AA29" s="5"/>
@@ -3856,12 +3912,12 @@
       <c r="T30" s="5">
         <v>1</v>
       </c>
-      <c r="U30" s="5" t="s">
+      <c r="U30" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V30" s="5"/>
       <c r="W30" s="5"/>
-      <c r="X30" s="5"/>
+      <c r="X30" s="17"/>
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
       <c r="AA30" s="5"/>
@@ -3948,12 +4004,12 @@
       <c r="T31" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U31" s="5" t="s">
+      <c r="U31" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V31" s="5"/>
       <c r="W31" s="5"/>
-      <c r="X31" s="5"/>
+      <c r="X31" s="17"/>
       <c r="Y31" s="5"/>
       <c r="Z31" s="5"/>
       <c r="AA31" s="5"/>
@@ -4040,12 +4096,12 @@
       <c r="T32" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="U32" s="11" t="s">
+      <c r="U32" s="19" t="s">
         <v>90</v>
       </c>
       <c r="V32" s="11"/>
       <c r="W32" s="11"/>
-      <c r="X32" s="11"/>
+      <c r="X32" s="19"/>
       <c r="Y32" s="11"/>
       <c r="Z32" s="11"/>
       <c r="AA32" s="11"/>
@@ -4132,12 +4188,12 @@
       <c r="T33" s="9">
         <v>1</v>
       </c>
-      <c r="U33" s="9" t="s">
+      <c r="U33" s="18" t="s">
         <v>78</v>
       </c>
       <c r="V33" s="9"/>
       <c r="W33" s="9"/>
-      <c r="X33" s="9"/>
+      <c r="X33" s="18"/>
       <c r="Y33" s="9"/>
       <c r="Z33" s="9"/>
       <c r="AA33" s="9"/>
@@ -4224,12 +4280,12 @@
       <c r="T34" s="5">
         <v>1</v>
       </c>
-      <c r="U34" s="5" t="s">
+      <c r="U34" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V34" s="5"/>
       <c r="W34" s="5"/>
-      <c r="X34" s="5"/>
+      <c r="X34" s="17"/>
       <c r="Y34" s="5"/>
       <c r="Z34" s="5"/>
       <c r="AA34" s="5"/>
@@ -4316,11 +4372,11 @@
       <c r="T35" s="5">
         <v>1</v>
       </c>
-      <c r="U35" s="5" t="s">
+      <c r="U35" s="17" t="s">
         <v>111</v>
       </c>
       <c r="W35" s="5"/>
-      <c r="X35" s="5"/>
+      <c r="X35" s="17"/>
       <c r="Y35" s="5"/>
       <c r="Z35" s="5"/>
       <c r="AA35" s="5"/>
@@ -4407,12 +4463,12 @@
       <c r="T36" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="U36" s="11" t="s">
+      <c r="U36" s="19" t="s">
         <v>90</v>
       </c>
       <c r="V36" s="11"/>
       <c r="W36" s="11"/>
-      <c r="X36" s="11"/>
+      <c r="X36" s="19"/>
       <c r="Y36" s="11"/>
       <c r="Z36" s="11"/>
       <c r="AA36" s="11"/>
@@ -4499,12 +4555,14 @@
       <c r="T37" s="5">
         <v>1</v>
       </c>
-      <c r="U37" s="5" t="s">
+      <c r="U37" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V37" s="5"/>
       <c r="W37" s="5"/>
-      <c r="X37" s="5"/>
+      <c r="X37" s="17" t="s">
+        <v>176</v>
+      </c>
       <c r="Y37" s="5"/>
       <c r="Z37" s="5"/>
       <c r="AA37" s="5"/>
@@ -4591,12 +4649,11 @@
       <c r="T38" s="5">
         <v>1</v>
       </c>
-      <c r="U38" s="5" t="s">
+      <c r="U38" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V38" s="5"/>
       <c r="W38" s="5"/>
-      <c r="X38" s="5"/>
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
       <c r="AA38" s="5"/>
@@ -4683,12 +4740,14 @@
       <c r="T39" s="5">
         <v>1</v>
       </c>
-      <c r="U39" s="5" t="s">
+      <c r="U39" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V39" s="5"/>
       <c r="W39" s="5"/>
-      <c r="X39" s="5"/>
+      <c r="X39" s="17" t="s">
+        <v>178</v>
+      </c>
       <c r="Y39" s="5"/>
       <c r="Z39" s="5"/>
       <c r="AA39" s="5"/>
@@ -4775,12 +4834,12 @@
       <c r="T40" s="5">
         <v>0</v>
       </c>
-      <c r="U40" s="5" t="s">
+      <c r="U40" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V40" s="5"/>
       <c r="W40" s="5"/>
-      <c r="X40" s="5"/>
+      <c r="X40" s="17"/>
       <c r="Y40" s="5"/>
       <c r="Z40" s="5"/>
       <c r="AA40" s="5"/>
@@ -4867,12 +4926,14 @@
       <c r="T41" s="5">
         <v>0</v>
       </c>
-      <c r="U41" s="5" t="s">
+      <c r="U41" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V41" s="5"/>
       <c r="W41" s="5"/>
-      <c r="X41" s="5"/>
+      <c r="X41" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="Y41" s="5"/>
       <c r="Z41" s="5"/>
       <c r="AA41" s="5"/>
@@ -4959,12 +5020,12 @@
       <c r="T42" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U42" s="5" t="s">
+      <c r="U42" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V42" s="5"/>
       <c r="W42" s="5"/>
-      <c r="X42" s="5"/>
+      <c r="X42" s="17"/>
       <c r="Y42" s="5"/>
       <c r="Z42" s="5"/>
       <c r="AA42" s="5"/>
@@ -5051,12 +5112,12 @@
       <c r="T43" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U43" s="5" t="s">
+      <c r="U43" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V43" s="5"/>
       <c r="W43" s="5"/>
-      <c r="X43" s="5"/>
+      <c r="X43" s="17"/>
       <c r="Y43" s="5"/>
       <c r="Z43" s="5"/>
       <c r="AA43" s="5"/>
@@ -5143,12 +5204,12 @@
       <c r="T44" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U44" s="5" t="s">
+      <c r="U44" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V44" s="5"/>
       <c r="W44" s="5"/>
-      <c r="X44" s="5"/>
+      <c r="X44" s="17"/>
       <c r="Y44" s="5"/>
       <c r="Z44" s="5"/>
       <c r="AA44" s="5"/>
@@ -5235,12 +5296,12 @@
       <c r="T45" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U45" s="5" t="s">
+      <c r="U45" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V45" s="5"/>
       <c r="W45" s="5"/>
-      <c r="X45" s="5"/>
+      <c r="X45" s="17"/>
       <c r="Y45" s="5"/>
       <c r="Z45" s="5"/>
       <c r="AA45" s="5"/>
@@ -5327,12 +5388,12 @@
       <c r="T46" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U46" s="5" t="s">
+      <c r="U46" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V46" s="5"/>
       <c r="W46" s="5"/>
-      <c r="X46" s="5"/>
+      <c r="X46" s="17"/>
       <c r="Y46" s="5"/>
       <c r="Z46" s="5"/>
       <c r="AA46" s="5"/>
@@ -5419,12 +5480,14 @@
       <c r="T47" s="5">
         <v>1</v>
       </c>
-      <c r="U47" s="5" t="s">
+      <c r="U47" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V47" s="5"/>
       <c r="W47" s="5"/>
-      <c r="X47" s="5"/>
+      <c r="X47" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="Y47" s="5"/>
       <c r="Z47" s="5"/>
       <c r="AA47" s="5"/>
@@ -5511,12 +5574,12 @@
       <c r="T48" s="5">
         <v>1</v>
       </c>
-      <c r="U48" s="5" t="s">
+      <c r="U48" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V48" s="5"/>
       <c r="W48" s="5"/>
-      <c r="X48" s="5"/>
+      <c r="X48" s="17"/>
       <c r="Y48" s="5"/>
       <c r="Z48" s="5"/>
       <c r="AA48" s="5"/>
@@ -5603,12 +5666,12 @@
       <c r="T49" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="U49" s="11" t="s">
+      <c r="U49" s="19" t="s">
         <v>90</v>
       </c>
       <c r="V49" s="11"/>
       <c r="W49" s="11"/>
-      <c r="X49" s="11"/>
+      <c r="X49" s="19"/>
       <c r="Y49" s="11"/>
       <c r="Z49" s="11"/>
       <c r="AA49" s="11"/>
@@ -5695,12 +5758,12 @@
       <c r="T50" s="5">
         <v>1</v>
       </c>
-      <c r="U50" s="5" t="s">
+      <c r="U50" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V50" s="5"/>
       <c r="W50" s="5"/>
-      <c r="X50" s="5"/>
+      <c r="X50" s="17"/>
       <c r="Y50" s="5"/>
       <c r="Z50" s="5"/>
       <c r="AA50" s="5"/>
@@ -5787,12 +5850,12 @@
       <c r="T51" s="5">
         <v>0</v>
       </c>
-      <c r="U51" s="5" t="s">
+      <c r="U51" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V51" s="5"/>
       <c r="W51" s="5"/>
-      <c r="X51" s="5"/>
+      <c r="X51" s="17"/>
       <c r="Y51" s="5"/>
       <c r="Z51" s="5"/>
       <c r="AA51" s="5"/>
@@ -5879,12 +5942,12 @@
       <c r="T52" s="5">
         <v>1</v>
       </c>
-      <c r="U52" s="5" t="s">
+      <c r="U52" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V52" s="5"/>
       <c r="W52" s="5"/>
-      <c r="X52" s="5"/>
+      <c r="X52" s="17"/>
       <c r="Y52" s="5"/>
       <c r="Z52" s="5"/>
       <c r="AA52" s="5"/>
@@ -5971,12 +6034,12 @@
       <c r="T53" s="5">
         <v>1</v>
       </c>
-      <c r="U53" s="5" t="s">
+      <c r="U53" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V53" s="5"/>
       <c r="W53" s="5"/>
-      <c r="X53" s="5"/>
+      <c r="X53" s="17"/>
       <c r="Y53" s="5"/>
       <c r="Z53" s="5"/>
       <c r="AA53" s="5"/>
@@ -6063,12 +6126,12 @@
       <c r="T54" s="5">
         <v>1</v>
       </c>
-      <c r="U54" s="5" t="s">
+      <c r="U54" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V54" s="5"/>
       <c r="W54" s="5"/>
-      <c r="X54" s="5"/>
+      <c r="X54" s="17"/>
       <c r="Y54" s="5"/>
       <c r="Z54" s="5"/>
       <c r="AA54" s="5"/>
@@ -6155,12 +6218,12 @@
       <c r="T55" s="5">
         <v>1</v>
       </c>
-      <c r="U55" s="5" t="s">
+      <c r="U55" s="17" t="s">
         <v>132</v>
       </c>
       <c r="V55" s="5"/>
       <c r="W55" s="5"/>
-      <c r="X55" s="5"/>
+      <c r="X55" s="17"/>
       <c r="Y55" s="5"/>
       <c r="Z55" s="5"/>
       <c r="AA55" s="5"/>
@@ -6247,12 +6310,12 @@
       <c r="T56" s="5">
         <v>1</v>
       </c>
-      <c r="U56" s="5" t="s">
+      <c r="U56" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V56" s="5"/>
       <c r="W56" s="5"/>
-      <c r="X56" s="5"/>
+      <c r="X56" s="17"/>
       <c r="Y56" s="5"/>
       <c r="Z56" s="5"/>
       <c r="AA56" s="5"/>
@@ -6339,12 +6402,12 @@
       <c r="T57" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="U57" s="11" t="s">
+      <c r="U57" s="19" t="s">
         <v>90</v>
       </c>
       <c r="V57" s="11"/>
       <c r="W57" s="11"/>
-      <c r="X57" s="11"/>
+      <c r="X57" s="19"/>
       <c r="Y57" s="11"/>
       <c r="Z57" s="11"/>
       <c r="AA57" s="11"/>
@@ -6431,12 +6494,12 @@
       <c r="T58" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="U58" s="11" t="s">
+      <c r="U58" s="19" t="s">
         <v>90</v>
       </c>
       <c r="V58" s="11"/>
       <c r="W58" s="11"/>
-      <c r="X58" s="11"/>
+      <c r="X58" s="19"/>
       <c r="Y58" s="11"/>
       <c r="Z58" s="11"/>
       <c r="AA58" s="11"/>
@@ -6523,12 +6586,12 @@
       <c r="T59" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="U59" s="13" t="s">
+      <c r="U59" s="20" t="s">
         <v>90</v>
       </c>
       <c r="V59" s="13"/>
       <c r="W59" s="13"/>
-      <c r="X59" s="13"/>
+      <c r="X59" s="20"/>
       <c r="Y59" s="13"/>
       <c r="Z59" s="13"/>
       <c r="AA59" s="13"/>
@@ -6615,12 +6678,12 @@
       <c r="T60" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="U60" s="11" t="s">
+      <c r="U60" s="19" t="s">
         <v>90</v>
       </c>
       <c r="V60" s="11"/>
       <c r="W60" s="11"/>
-      <c r="X60" s="11"/>
+      <c r="X60" s="19"/>
       <c r="Y60" s="11"/>
       <c r="Z60" s="11"/>
       <c r="AA60" s="11"/>
@@ -6707,12 +6770,12 @@
       <c r="T61" s="9">
         <v>1</v>
       </c>
-      <c r="U61" s="9" t="s">
+      <c r="U61" s="18" t="s">
         <v>78</v>
       </c>
       <c r="V61" s="9"/>
       <c r="W61" s="9"/>
-      <c r="X61" s="9"/>
+      <c r="X61" s="18"/>
       <c r="Y61" s="9"/>
       <c r="Z61" s="9"/>
       <c r="AA61" s="9"/>
@@ -6799,12 +6862,12 @@
       <c r="T62" s="5">
         <v>0</v>
       </c>
-      <c r="U62" s="5" t="s">
+      <c r="U62" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V62" s="5"/>
       <c r="W62" s="5"/>
-      <c r="X62" s="5"/>
+      <c r="X62" s="17"/>
       <c r="Y62" s="5"/>
       <c r="Z62" s="5"/>
       <c r="AA62" s="5"/>
@@ -6891,12 +6954,12 @@
       <c r="T63" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="U63" s="11" t="s">
+      <c r="U63" s="19" t="s">
         <v>90</v>
       </c>
       <c r="V63" s="11"/>
       <c r="W63" s="11"/>
-      <c r="X63" s="11"/>
+      <c r="X63" s="19"/>
       <c r="Y63" s="11"/>
       <c r="Z63" s="11"/>
       <c r="AA63" s="11"/>
@@ -6983,12 +7046,12 @@
       <c r="T64" s="5">
         <v>0</v>
       </c>
-      <c r="U64" s="5" t="s">
+      <c r="U64" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V64" s="5"/>
       <c r="W64" s="5"/>
-      <c r="X64" s="5"/>
+      <c r="X64" s="17"/>
       <c r="Y64" s="5"/>
       <c r="Z64" s="5"/>
       <c r="AA64" s="5"/>
@@ -7075,12 +7138,12 @@
       <c r="T65" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="U65" s="11" t="s">
+      <c r="U65" s="19" t="s">
         <v>90</v>
       </c>
       <c r="V65" s="11"/>
       <c r="W65" s="11"/>
-      <c r="X65" s="11"/>
+      <c r="X65" s="19"/>
       <c r="Y65" s="11"/>
       <c r="Z65" s="11"/>
       <c r="AA65" s="11"/>
@@ -7167,12 +7230,12 @@
       <c r="T66" s="5">
         <v>0</v>
       </c>
-      <c r="U66" s="5" t="s">
+      <c r="U66" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V66" s="5"/>
       <c r="W66" s="5"/>
-      <c r="X66" s="5"/>
+      <c r="X66" s="17"/>
       <c r="Y66" s="5"/>
       <c r="Z66" s="5"/>
       <c r="AA66" s="5"/>
@@ -7259,12 +7322,14 @@
       <c r="T67" s="5">
         <v>1</v>
       </c>
-      <c r="U67" s="5" t="s">
+      <c r="U67" s="17" t="s">
         <v>132</v>
       </c>
       <c r="V67" s="5"/>
       <c r="W67" s="5"/>
-      <c r="X67" s="5"/>
+      <c r="X67" s="17" t="s">
+        <v>171</v>
+      </c>
       <c r="Y67" s="5"/>
       <c r="Z67" s="5"/>
       <c r="AA67" s="5"/>
@@ -7351,12 +7416,12 @@
       <c r="T68" s="5">
         <v>0</v>
       </c>
-      <c r="U68" s="5" t="s">
+      <c r="U68" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V68" s="5"/>
       <c r="W68" s="5"/>
-      <c r="X68" s="5"/>
+      <c r="X68" s="17"/>
       <c r="Y68" s="5"/>
       <c r="Z68" s="5"/>
       <c r="AA68" s="5"/>
@@ -7443,12 +7508,12 @@
       <c r="T69" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U69" s="5" t="s">
+      <c r="U69" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V69" s="5"/>
       <c r="W69" s="5"/>
-      <c r="X69" s="5"/>
+      <c r="X69" s="17"/>
       <c r="Y69" s="5"/>
       <c r="Z69" s="5"/>
       <c r="AA69" s="5"/>
@@ -7535,12 +7600,14 @@
       <c r="T70" s="5">
         <v>1</v>
       </c>
-      <c r="U70" s="5" t="s">
+      <c r="U70" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V70" s="5"/>
       <c r="W70" s="5"/>
-      <c r="X70" s="5"/>
+      <c r="X70" s="17" t="s">
+        <v>172</v>
+      </c>
       <c r="Y70" s="5"/>
       <c r="Z70" s="5"/>
       <c r="AA70" s="5"/>
@@ -7627,12 +7694,14 @@
       <c r="T71" s="5">
         <v>0</v>
       </c>
-      <c r="U71" s="5" t="s">
+      <c r="U71" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V71" s="5"/>
       <c r="W71" s="5"/>
-      <c r="X71" s="5"/>
+      <c r="X71" s="17" t="s">
+        <v>173</v>
+      </c>
       <c r="Y71" s="5"/>
       <c r="Z71" s="5"/>
       <c r="AA71" s="5"/>
@@ -7719,12 +7788,14 @@
       <c r="T72" s="5">
         <v>1</v>
       </c>
-      <c r="U72" s="5" t="s">
+      <c r="U72" s="17" t="s">
         <v>151</v>
       </c>
       <c r="V72" s="5"/>
       <c r="W72" s="5"/>
-      <c r="X72" s="5"/>
+      <c r="X72" s="17" t="s">
+        <v>174</v>
+      </c>
       <c r="Y72" s="5"/>
       <c r="Z72" s="5"/>
       <c r="AA72" s="5"/>
@@ -7811,12 +7882,14 @@
       <c r="T73" s="5">
         <v>1</v>
       </c>
-      <c r="U73" s="5" t="s">
+      <c r="U73" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V73" s="5"/>
       <c r="W73" s="5"/>
-      <c r="X73" s="5"/>
+      <c r="X73" s="17" t="s">
+        <v>175</v>
+      </c>
       <c r="Y73" s="5"/>
       <c r="Z73" s="5"/>
       <c r="AA73" s="5"/>
@@ -7903,12 +7976,12 @@
       <c r="T74" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="U74" s="11" t="s">
+      <c r="U74" s="19" t="s">
         <v>90</v>
       </c>
       <c r="V74" s="11"/>
       <c r="W74" s="11"/>
-      <c r="X74" s="11"/>
+      <c r="X74" s="19"/>
       <c r="Y74" s="11"/>
       <c r="Z74" s="11"/>
       <c r="AA74" s="11"/>
@@ -7995,12 +8068,12 @@
       <c r="T75" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U75" s="5" t="s">
+      <c r="U75" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V75" s="5"/>
       <c r="W75" s="5"/>
-      <c r="X75" s="5"/>
+      <c r="X75" s="17"/>
       <c r="Y75" s="5"/>
       <c r="Z75" s="5"/>
       <c r="AA75" s="5"/>
@@ -8087,12 +8160,12 @@
       <c r="T76" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U76" s="5" t="s">
+      <c r="U76" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V76" s="5"/>
       <c r="W76" s="5"/>
-      <c r="X76" s="5"/>
+      <c r="X76" s="17"/>
       <c r="Y76" s="5"/>
       <c r="Z76" s="5"/>
       <c r="AA76" s="5"/>
@@ -8179,12 +8252,12 @@
       <c r="T77" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U77" s="5" t="s">
+      <c r="U77" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V77" s="5"/>
       <c r="W77" s="5"/>
-      <c r="X77" s="5"/>
+      <c r="X77" s="17"/>
       <c r="Y77" s="5"/>
       <c r="Z77" s="5"/>
       <c r="AA77" s="5"/>
@@ -8271,12 +8344,12 @@
       <c r="T78" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U78" s="5" t="s">
+      <c r="U78" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V78" s="5"/>
       <c r="W78" s="5"/>
-      <c r="X78" s="5"/>
+      <c r="X78" s="17"/>
       <c r="Y78" s="5"/>
       <c r="Z78" s="5"/>
       <c r="AA78" s="5"/>
@@ -8363,12 +8436,12 @@
       <c r="T79" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U79" s="5" t="s">
+      <c r="U79" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V79" s="5"/>
       <c r="W79" s="5"/>
-      <c r="X79" s="5"/>
+      <c r="X79" s="17"/>
       <c r="Y79" s="5"/>
       <c r="Z79" s="5"/>
       <c r="AA79" s="5"/>
@@ -8455,12 +8528,12 @@
       <c r="T80" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U80" s="5" t="s">
+      <c r="U80" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V80" s="5"/>
       <c r="W80" s="5"/>
-      <c r="X80" s="5"/>
+      <c r="X80" s="17"/>
       <c r="Y80" s="5"/>
       <c r="Z80" s="5"/>
       <c r="AA80" s="5"/>
@@ -8547,12 +8620,12 @@
       <c r="T81" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U81" s="5" t="s">
+      <c r="U81" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V81" s="5"/>
       <c r="W81" s="5"/>
-      <c r="X81" s="5"/>
+      <c r="X81" s="17"/>
       <c r="Y81" s="5"/>
       <c r="Z81" s="5"/>
       <c r="AA81" s="5"/>
@@ -8639,12 +8712,12 @@
       <c r="T82" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U82" s="5" t="s">
+      <c r="U82" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V82" s="5"/>
       <c r="W82" s="5"/>
-      <c r="X82" s="5"/>
+      <c r="X82" s="17"/>
       <c r="Y82" s="5"/>
       <c r="Z82" s="5"/>
       <c r="AA82" s="5"/>
@@ -8731,12 +8804,12 @@
       <c r="T83" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="U83" s="11" t="s">
+      <c r="U83" s="19" t="s">
         <v>90</v>
       </c>
       <c r="V83" s="11"/>
       <c r="W83" s="11"/>
-      <c r="X83" s="11"/>
+      <c r="X83" s="19"/>
       <c r="Y83" s="11"/>
       <c r="Z83" s="11"/>
       <c r="AA83" s="11"/>
@@ -8823,12 +8896,12 @@
       <c r="T84" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U84" s="5" t="s">
+      <c r="U84" s="17" t="s">
         <v>90</v>
       </c>
       <c r="V84" s="5"/>
       <c r="W84" s="5"/>
-      <c r="X84" s="5"/>
+      <c r="X84" s="17"/>
       <c r="Y84" s="5"/>
       <c r="Z84" s="5"/>
       <c r="AA84" s="5"/>
@@ -8915,12 +8988,12 @@
       <c r="T85" s="5">
         <v>1</v>
       </c>
-      <c r="U85" s="5" t="s">
+      <c r="U85" s="17" t="s">
         <v>78</v>
       </c>
       <c r="V85" s="5"/>
       <c r="W85" s="5"/>
-      <c r="X85" s="5"/>
+      <c r="X85" s="17"/>
       <c r="Y85" s="5"/>
       <c r="Z85" s="5"/>
       <c r="AA85" s="16"/>

</xml_diff>

<commit_message>
Fixed subs 004, 010, 012, 028, 054, 069, 071, fixed T-peak, added new subs
</commit_message>
<xml_diff>
--- a/meta/MEG_ANALYSIS_MASTERFILE.xlsx
+++ b/meta/MEG_ANALYSIS_MASTERFILE.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\meditation\ERC\Analyses\MEG\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782C9F0B-C79B-456E-9D96-2F3D088A89F8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CE166E-8D37-41BB-BD9A-62B51F3A4B93}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4095" windowHeight="9000" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MEG_ANALYSIS_MASTERFILE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="184">
   <si>
     <t>ANATOMY</t>
   </si>
@@ -562,10 +562,22 @@
     <t>MRT41|MRT51|MRT52</t>
   </si>
   <si>
-    <t>MLF11|MLF12|MLF13|MLF14|MLT21|MLT31|MLT32|MLT41|MLT42|MLT51|MLT52</t>
-  </si>
-  <si>
     <t>MLT41|MLT42|MLT43|MLT44|MLT51|MLT52|MLT53|MLT54</t>
+  </si>
+  <si>
+    <t>MLF11|MLF12|MLF13|MLF14|MLF21|MLF22|MLF23|MLF24|MLF25|MLT21|MLT31|MLT32|MLT41|MLT42|MLT51|MLT52|MRF11|MRF12|MRF13|MRF14|MRF21|MRF22|MRF23|MRF24|MRF25|MRT21|MRT31|MRT32|MRT41|MRT42|MRT51|MRT52|MZF01</t>
+  </si>
+  <si>
+    <t>MLF11|MLF12|MLF13|MLF14|MLF21|MLF22|MLF23|MLF24|MLF25|MLT11|MLT21|MLT22|MLT31|MLT32|MLT33|MLT41|MLT42|MLT43|MLT51|MLT52|MLT53|MRF11|MRF12|MRF13|MRF14|MRF21|MRF22|MRF23|MRF24|MRF25|MRT11|MRT21|MRT22|MRT31|MRT32|MRT33|MRT41|MRT42|MRT43|MRT51|MRT52|MRT53|MZF01</t>
+  </si>
+  <si>
+    <t>EEG001|EEG002|EEG003|EEG004|EEG005|EEG006|EEG007|EEG009</t>
+  </si>
+  <si>
+    <t>EEG003|EEG004|EEG005|EEG006|EEG007|EEG008</t>
+  </si>
+  <si>
+    <t>EEG005|EEG006|EEG007|EEG008</t>
   </si>
 </sst>
 </file>
@@ -690,7 +702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -752,12 +764,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -768,6 +774,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1155,10 +1173,10 @@
   <dimension ref="A1:AZ85"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="O30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="X41" sqref="X41"/>
+      <selection pane="bottomRight" activeCell="AB76" sqref="AB76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1170,64 +1188,64 @@
     <row r="1" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
+      <c r="J1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
       <c r="Y1" s="1"/>
-      <c r="Z1" s="26" t="s">
+      <c r="Z1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
-      <c r="AI1" s="26"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
       <c r="AJ1" s="1"/>
-      <c r="AK1" s="26" t="s">
+      <c r="AK1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="26"/>
-      <c r="AM1" s="26"/>
-      <c r="AN1" s="26"/>
-      <c r="AO1" s="26"/>
-      <c r="AP1" s="26"/>
-      <c r="AQ1" s="26"/>
-      <c r="AR1" s="26"/>
-      <c r="AS1" s="26"/>
-      <c r="AT1" s="26"/>
-      <c r="AU1" s="26"/>
-      <c r="AV1" s="26"/>
-      <c r="AW1" s="26"/>
-      <c r="AX1" s="26"/>
-      <c r="AY1" s="26"/>
-      <c r="AZ1" s="26"/>
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="24"/>
+      <c r="AP1" s="24"/>
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="24"/>
+      <c r="AT1" s="24"/>
+      <c r="AU1" s="24"/>
+      <c r="AV1" s="24"/>
+      <c r="AW1" s="24"/>
+      <c r="AX1" s="24"/>
+      <c r="AY1" s="24"/>
+      <c r="AZ1" s="24"/>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A2" s="22" t="s">
@@ -1241,32 +1259,32 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24" t="s">
+      <c r="K2" s="27"/>
+      <c r="L2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24" t="s">
+      <c r="M2" s="28"/>
+      <c r="N2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24" t="s">
+      <c r="O2" s="28"/>
+      <c r="P2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
       <c r="S2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="27" t="s">
+      <c r="T2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
       <c r="X2" s="3" t="s">
         <v>167</v>
       </c>
@@ -1274,21 +1292,21 @@
       <c r="Z2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="28" t="s">
+      <c r="AA2" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="28" t="s">
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="AE2" s="28"/>
-      <c r="AF2" s="28"/>
-      <c r="AG2" s="28" t="s">
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
+      <c r="AG2" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
+      <c r="AH2" s="26"/>
+      <c r="AI2" s="26"/>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1" t="s">
         <v>15</v>
@@ -1649,97 +1667,97 @@
       <c r="AY5" s="5"/>
       <c r="AZ5" s="5"/>
     </row>
-    <row r="6" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:52" s="14" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9">
-        <v>1</v>
-      </c>
-      <c r="E6" s="9">
-        <v>1</v>
-      </c>
-      <c r="F6" s="9">
-        <v>0</v>
-      </c>
-      <c r="G6" s="9">
-        <v>1</v>
-      </c>
-      <c r="H6" s="9">
-        <v>1</v>
-      </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9" t="s">
+      <c r="C6" s="13">
+        <v>1</v>
+      </c>
+      <c r="D6" s="13">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>1</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9" t="s">
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9" t="s">
+      <c r="O6" s="13"/>
+      <c r="P6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="S6" s="9" t="s">
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="S6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="T6" s="9">
-        <v>1</v>
-      </c>
-      <c r="U6" s="18" t="s">
+      <c r="T6" s="13">
+        <v>1</v>
+      </c>
+      <c r="U6" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9">
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13">
         <v>-1</v>
       </c>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
-      <c r="AE6" s="9">
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="13">
         <v>-1</v>
       </c>
-      <c r="AF6" s="9"/>
-      <c r="AG6" s="9"/>
-      <c r="AH6" s="9">
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="13">
         <v>-1</v>
       </c>
-      <c r="AI6" s="9"/>
-      <c r="AJ6" s="9"/>
-      <c r="AK6" s="9"/>
-      <c r="AL6" s="9"/>
-      <c r="AM6" s="9"/>
-      <c r="AN6" s="9"/>
-      <c r="AO6" s="9"/>
-      <c r="AP6" s="9"/>
-      <c r="AQ6" s="9"/>
-      <c r="AR6" s="9"/>
-      <c r="AS6" s="9"/>
-      <c r="AT6" s="9"/>
-      <c r="AU6" s="9"/>
-      <c r="AV6" s="9"/>
-      <c r="AW6" s="9"/>
-      <c r="AX6" s="9"/>
-      <c r="AY6" s="9"/>
-      <c r="AZ6" s="9"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13"/>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="13"/>
+      <c r="AN6" s="13"/>
+      <c r="AO6" s="13"/>
+      <c r="AP6" s="13"/>
+      <c r="AQ6" s="13"/>
+      <c r="AR6" s="13"/>
+      <c r="AS6" s="13"/>
+      <c r="AT6" s="13"/>
+      <c r="AU6" s="13"/>
+      <c r="AV6" s="13"/>
+      <c r="AW6" s="13"/>
+      <c r="AX6" s="13"/>
+      <c r="AY6" s="13"/>
+      <c r="AZ6" s="13"/>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
@@ -4598,96 +4616,97 @@
       <c r="AY37" s="5"/>
       <c r="AZ37" s="5"/>
     </row>
-    <row r="38" spans="1:52" x14ac:dyDescent="0.45">
-      <c r="A38" s="5" t="s">
+    <row r="38" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C38" s="5">
-        <v>1</v>
-      </c>
-      <c r="D38" s="5">
-        <v>1</v>
-      </c>
-      <c r="E38" s="5">
-        <v>1</v>
-      </c>
-      <c r="F38" s="5">
-        <v>1</v>
-      </c>
-      <c r="G38" s="5">
-        <v>1</v>
-      </c>
-      <c r="H38" s="5">
-        <v>1</v>
-      </c>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5" t="s">
+      <c r="C38" s="9">
+        <v>1</v>
+      </c>
+      <c r="D38" s="9">
+        <v>1</v>
+      </c>
+      <c r="E38" s="9">
+        <v>1</v>
+      </c>
+      <c r="F38" s="9">
+        <v>1</v>
+      </c>
+      <c r="G38" s="9">
+        <v>1</v>
+      </c>
+      <c r="H38" s="9">
+        <v>1</v>
+      </c>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K38" s="5" t="s">
+      <c r="K38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5" t="s">
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5" t="s">
+      <c r="O38" s="9"/>
+      <c r="P38" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="Q38" s="5"/>
-      <c r="R38" s="5" t="s">
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="S38" s="5" t="s">
+      <c r="S38" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="T38" s="5">
-        <v>1</v>
-      </c>
-      <c r="U38" s="17" t="s">
+      <c r="T38" s="9">
+        <v>1</v>
+      </c>
+      <c r="U38" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="V38" s="5"/>
-      <c r="W38" s="5"/>
-      <c r="Y38" s="5"/>
-      <c r="Z38" s="5"/>
-      <c r="AA38" s="5"/>
-      <c r="AB38" s="5">
-        <v>1</v>
-      </c>
-      <c r="AC38" s="5"/>
-      <c r="AD38" s="5"/>
-      <c r="AE38" s="5">
-        <v>1</v>
-      </c>
-      <c r="AF38" s="5"/>
-      <c r="AG38" s="5"/>
-      <c r="AH38" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI38" s="5"/>
-      <c r="AJ38" s="5"/>
-      <c r="AK38" s="5"/>
-      <c r="AL38" s="5"/>
-      <c r="AM38" s="5"/>
-      <c r="AN38" s="5"/>
-      <c r="AO38" s="5"/>
-      <c r="AP38" s="5"/>
-      <c r="AQ38" s="5"/>
-      <c r="AR38" s="5"/>
-      <c r="AS38" s="5"/>
-      <c r="AT38" s="5"/>
-      <c r="AU38" s="5"/>
-      <c r="AV38" s="5"/>
-      <c r="AW38" s="5"/>
-      <c r="AX38" s="5"/>
-      <c r="AY38" s="5"/>
-      <c r="AZ38" s="5"/>
+      <c r="V38" s="9"/>
+      <c r="W38" s="9"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="9"/>
+      <c r="Z38" s="9"/>
+      <c r="AA38" s="9"/>
+      <c r="AB38" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC38" s="9"/>
+      <c r="AD38" s="9"/>
+      <c r="AE38" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF38" s="9"/>
+      <c r="AG38" s="9"/>
+      <c r="AH38" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI38" s="9"/>
+      <c r="AJ38" s="9"/>
+      <c r="AK38" s="9"/>
+      <c r="AL38" s="9"/>
+      <c r="AM38" s="9"/>
+      <c r="AN38" s="9"/>
+      <c r="AO38" s="9"/>
+      <c r="AP38" s="9"/>
+      <c r="AQ38" s="9"/>
+      <c r="AR38" s="9"/>
+      <c r="AS38" s="9"/>
+      <c r="AT38" s="9"/>
+      <c r="AU38" s="9"/>
+      <c r="AV38" s="9"/>
+      <c r="AW38" s="9"/>
+      <c r="AX38" s="9"/>
+      <c r="AY38" s="9"/>
+      <c r="AZ38" s="9"/>
     </row>
     <row r="39" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A39" s="5" t="s">
@@ -4746,7 +4765,7 @@
       <c r="V39" s="5"/>
       <c r="W39" s="5"/>
       <c r="X39" s="17" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="Y39" s="5"/>
       <c r="Z39" s="5"/>
@@ -4932,7 +4951,7 @@
       <c r="V41" s="5"/>
       <c r="W41" s="5"/>
       <c r="X41" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y41" s="5"/>
       <c r="Z41" s="5"/>
@@ -4973,7 +4992,7 @@
       <c r="A42" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="8" t="s">
         <v>118</v>
       </c>
       <c r="C42" s="5">
@@ -4985,42 +5004,42 @@
       <c r="E42" s="5">
         <v>0</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>90</v>
+      <c r="F42" s="5">
+        <v>0</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0</v>
+      </c>
+      <c r="H42" s="5">
+        <v>0</v>
       </c>
       <c r="I42" s="5"/>
       <c r="J42" s="5" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
       <c r="N42" s="5" t="s">
-        <v>90</v>
+        <v>165</v>
       </c>
       <c r="O42" s="5"/>
       <c r="P42" s="5" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="Q42" s="5"/>
       <c r="R42" s="5" t="s">
         <v>90</v>
       </c>
       <c r="S42" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="T42" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="U42" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="T42" s="5">
+        <v>0</v>
+      </c>
+      <c r="U42" s="21" t="s">
         <v>90</v>
       </c>
       <c r="V42" s="5"/>
@@ -5029,18 +5048,18 @@
       <c r="Y42" s="5"/>
       <c r="Z42" s="5"/>
       <c r="AA42" s="5"/>
-      <c r="AB42" s="5" t="s">
-        <v>90</v>
+      <c r="AB42" s="5">
+        <v>0</v>
       </c>
       <c r="AC42" s="5"/>
       <c r="AD42" s="5"/>
-      <c r="AE42" s="5" t="s">
-        <v>90</v>
+      <c r="AE42" s="5">
+        <v>0</v>
       </c>
       <c r="AF42" s="5"/>
       <c r="AG42" s="5"/>
-      <c r="AH42" s="5" t="s">
-        <v>90</v>
+      <c r="AH42" s="5">
+        <v>0</v>
       </c>
       <c r="AI42" s="5"/>
       <c r="AJ42" s="5"/>
@@ -5065,7 +5084,7 @@
       <c r="A43" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="8" t="s">
         <v>119</v>
       </c>
       <c r="C43" s="5">
@@ -5077,43 +5096,43 @@
       <c r="E43" s="5">
         <v>0</v>
       </c>
-      <c r="F43" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>90</v>
+      <c r="F43" s="5">
+        <v>0</v>
+      </c>
+      <c r="G43" s="5">
+        <v>0</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0</v>
       </c>
       <c r="I43" s="5"/>
       <c r="J43" s="5" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5" t="s">
-        <v>90</v>
+        <v>165</v>
       </c>
       <c r="O43" s="5"/>
       <c r="P43" s="5" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="Q43" s="5"/>
       <c r="R43" s="5" t="s">
         <v>90</v>
       </c>
       <c r="S43" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="T43" s="5" t="s">
-        <v>90</v>
+        <v>30</v>
+      </c>
+      <c r="T43" s="5">
+        <v>1</v>
       </c>
       <c r="U43" s="17" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="V43" s="5"/>
       <c r="W43" s="5"/>
@@ -5121,18 +5140,18 @@
       <c r="Y43" s="5"/>
       <c r="Z43" s="5"/>
       <c r="AA43" s="5"/>
-      <c r="AB43" s="5" t="s">
-        <v>90</v>
+      <c r="AB43" s="5">
+        <v>0</v>
       </c>
       <c r="AC43" s="5"/>
       <c r="AD43" s="5"/>
-      <c r="AE43" s="5" t="s">
-        <v>90</v>
+      <c r="AE43" s="5">
+        <v>0</v>
       </c>
       <c r="AF43" s="5"/>
       <c r="AG43" s="5"/>
-      <c r="AH43" s="5" t="s">
-        <v>90</v>
+      <c r="AH43" s="5">
+        <v>0</v>
       </c>
       <c r="AI43" s="5"/>
       <c r="AJ43" s="5"/>
@@ -5157,7 +5176,7 @@
       <c r="A44" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="8" t="s">
         <v>120</v>
       </c>
       <c r="C44" s="5">
@@ -5169,43 +5188,43 @@
       <c r="E44" s="5">
         <v>0</v>
       </c>
-      <c r="F44" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>90</v>
+      <c r="F44" s="5">
+        <v>0</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0</v>
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="L44" s="5"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5" t="s">
-        <v>90</v>
+        <v>165</v>
       </c>
       <c r="O44" s="5"/>
       <c r="P44" s="5" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="Q44" s="5"/>
       <c r="R44" s="5" t="s">
         <v>90</v>
       </c>
       <c r="S44" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="T44" s="5" t="s">
-        <v>90</v>
+        <v>28</v>
+      </c>
+      <c r="T44" s="5">
+        <v>1</v>
       </c>
       <c r="U44" s="17" t="s">
-        <v>90</v>
+        <v>181</v>
       </c>
       <c r="V44" s="5"/>
       <c r="W44" s="5"/>
@@ -5213,18 +5232,18 @@
       <c r="Y44" s="5"/>
       <c r="Z44" s="5"/>
       <c r="AA44" s="5"/>
-      <c r="AB44" s="5" t="s">
-        <v>90</v>
+      <c r="AB44" s="5">
+        <v>0</v>
       </c>
       <c r="AC44" s="5"/>
       <c r="AD44" s="5"/>
-      <c r="AE44" s="5" t="s">
-        <v>90</v>
+      <c r="AE44" s="5">
+        <v>0</v>
       </c>
       <c r="AF44" s="5"/>
       <c r="AG44" s="5"/>
-      <c r="AH44" s="5" t="s">
-        <v>90</v>
+      <c r="AH44" s="5">
+        <v>0</v>
       </c>
       <c r="AI44" s="5"/>
       <c r="AJ44" s="5"/>
@@ -5615,97 +5634,97 @@
       <c r="AY48" s="5"/>
       <c r="AZ48" s="5"/>
     </row>
-    <row r="49" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="11" t="s">
+    <row r="49" spans="1:52" s="14" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C49" s="11">
-        <v>0</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="K49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="S49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="T49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="U49" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="V49" s="11"/>
-      <c r="W49" s="11"/>
-      <c r="X49" s="19"/>
-      <c r="Y49" s="11"/>
-      <c r="Z49" s="11"/>
-      <c r="AA49" s="11"/>
-      <c r="AB49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC49" s="11"/>
-      <c r="AD49" s="11"/>
-      <c r="AE49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF49" s="11"/>
-      <c r="AG49" s="11"/>
-      <c r="AH49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI49" s="11"/>
-      <c r="AJ49" s="11"/>
-      <c r="AK49" s="11"/>
-      <c r="AL49" s="11"/>
-      <c r="AM49" s="11"/>
-      <c r="AN49" s="11"/>
-      <c r="AO49" s="11"/>
-      <c r="AP49" s="11"/>
-      <c r="AQ49" s="11"/>
-      <c r="AR49" s="11"/>
-      <c r="AS49" s="11"/>
-      <c r="AT49" s="11"/>
-      <c r="AU49" s="11"/>
-      <c r="AV49" s="11"/>
-      <c r="AW49" s="11"/>
-      <c r="AX49" s="11"/>
-      <c r="AY49" s="11"/>
-      <c r="AZ49" s="11"/>
+      <c r="C49" s="13">
+        <v>1</v>
+      </c>
+      <c r="D49" s="13">
+        <v>0</v>
+      </c>
+      <c r="E49" s="13">
+        <v>0</v>
+      </c>
+      <c r="F49" s="13">
+        <v>0</v>
+      </c>
+      <c r="G49" s="13">
+        <v>0</v>
+      </c>
+      <c r="H49" s="13">
+        <v>0</v>
+      </c>
+      <c r="I49" s="13"/>
+      <c r="J49" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="O49" s="13"/>
+      <c r="P49" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="S49" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T49" s="13">
+        <v>1</v>
+      </c>
+      <c r="U49" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="V49" s="13"/>
+      <c r="W49" s="13"/>
+      <c r="X49" s="20"/>
+      <c r="Y49" s="13"/>
+      <c r="Z49" s="13"/>
+      <c r="AA49" s="13"/>
+      <c r="AB49" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC49" s="13"/>
+      <c r="AD49" s="13"/>
+      <c r="AE49" s="13">
+        <v>0</v>
+      </c>
+      <c r="AF49" s="13"/>
+      <c r="AG49" s="13"/>
+      <c r="AH49" s="13">
+        <v>0</v>
+      </c>
+      <c r="AI49" s="13"/>
+      <c r="AJ49" s="13"/>
+      <c r="AK49" s="13"/>
+      <c r="AL49" s="13"/>
+      <c r="AM49" s="13"/>
+      <c r="AN49" s="13"/>
+      <c r="AO49" s="13"/>
+      <c r="AP49" s="13"/>
+      <c r="AQ49" s="13"/>
+      <c r="AR49" s="13"/>
+      <c r="AS49" s="13"/>
+      <c r="AT49" s="13"/>
+      <c r="AU49" s="13"/>
+      <c r="AV49" s="13"/>
+      <c r="AW49" s="13"/>
+      <c r="AX49" s="13"/>
+      <c r="AY49" s="13"/>
+      <c r="AZ49" s="13"/>
     </row>
     <row r="50" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A50" s="5" t="s">
@@ -6131,7 +6150,9 @@
       </c>
       <c r="V54" s="5"/>
       <c r="W54" s="5"/>
-      <c r="X54" s="17"/>
+      <c r="X54" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="Y54" s="5"/>
       <c r="Z54" s="5"/>
       <c r="AA54" s="5"/>
@@ -6171,11 +6192,11 @@
       <c r="A55" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C55" s="8">
-        <v>0</v>
+      <c r="C55" s="16">
+        <v>1</v>
       </c>
       <c r="D55" s="5">
         <v>0</v>
@@ -6542,8 +6563,8 @@
       <c r="B59" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C59" s="15">
-        <v>0</v>
+      <c r="C59" s="30">
+        <v>1</v>
       </c>
       <c r="D59" s="13" t="s">
         <v>90</v>
@@ -6595,18 +6616,18 @@
       <c r="Y59" s="13"/>
       <c r="Z59" s="13"/>
       <c r="AA59" s="13"/>
-      <c r="AB59" s="15">
-        <v>0</v>
+      <c r="AB59" s="15" t="s">
+        <v>90</v>
       </c>
       <c r="AC59" s="13"/>
       <c r="AD59" s="13"/>
-      <c r="AE59" s="15">
-        <v>0</v>
+      <c r="AE59" s="15" t="s">
+        <v>90</v>
       </c>
       <c r="AF59" s="13"/>
       <c r="AG59" s="13"/>
-      <c r="AH59" s="15">
-        <v>0</v>
+      <c r="AH59" s="15" t="s">
+        <v>90</v>
       </c>
       <c r="AI59" s="13"/>
       <c r="AJ59" s="13"/>
@@ -7461,55 +7482,55 @@
       <c r="A69" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C69" s="8">
-        <v>0</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H69" s="5" t="s">
-        <v>90</v>
+      <c r="C69" s="16">
+        <v>1</v>
+      </c>
+      <c r="D69" s="5">
+        <v>0</v>
+      </c>
+      <c r="E69" s="5">
+        <v>0</v>
+      </c>
+      <c r="F69" s="5">
+        <v>0</v>
+      </c>
+      <c r="G69" s="5">
+        <v>0</v>
+      </c>
+      <c r="H69" s="5">
+        <v>0</v>
       </c>
       <c r="I69" s="5"/>
       <c r="J69" s="5" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="K69" s="5" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="L69" s="5"/>
       <c r="M69" s="5"/>
       <c r="N69" s="5" t="s">
-        <v>90</v>
+        <v>165</v>
       </c>
       <c r="O69" s="5"/>
       <c r="P69" s="5" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="Q69" s="5"/>
       <c r="R69" s="5" t="s">
         <v>90</v>
       </c>
       <c r="S69" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="T69" s="5" t="s">
-        <v>90</v>
+        <v>30</v>
+      </c>
+      <c r="T69" s="5">
+        <v>1</v>
       </c>
       <c r="U69" s="17" t="s">
-        <v>90</v>
+        <v>181</v>
       </c>
       <c r="V69" s="5"/>
       <c r="W69" s="5"/>
@@ -7517,17 +7538,17 @@
       <c r="Y69" s="5"/>
       <c r="Z69" s="5"/>
       <c r="AA69" s="5"/>
-      <c r="AB69" s="8">
+      <c r="AB69" s="16">
         <v>0</v>
       </c>
       <c r="AC69" s="5"/>
       <c r="AD69" s="5"/>
-      <c r="AE69" s="8">
+      <c r="AE69" s="16">
         <v>0</v>
       </c>
       <c r="AF69" s="5"/>
       <c r="AG69" s="5"/>
-      <c r="AH69" s="8">
+      <c r="AH69" s="16">
         <v>0</v>
       </c>
       <c r="AI69" s="5"/>
@@ -8021,10 +8042,10 @@
       <c r="A75" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C75" s="8">
         <v>0</v>
       </c>
       <c r="D75" s="5" t="s">
@@ -8077,17 +8098,17 @@
       <c r="Y75" s="5"/>
       <c r="Z75" s="5"/>
       <c r="AA75" s="5"/>
-      <c r="AB75" s="8">
+      <c r="AB75" s="16">
         <v>0</v>
       </c>
       <c r="AC75" s="5"/>
       <c r="AD75" s="5"/>
-      <c r="AE75" s="8">
+      <c r="AE75" s="16">
         <v>0</v>
       </c>
       <c r="AF75" s="5"/>
       <c r="AG75" s="5"/>
-      <c r="AH75" s="8">
+      <c r="AH75" s="16">
         <v>0</v>
       </c>
       <c r="AI75" s="5"/>
@@ -8116,8 +8137,8 @@
       <c r="B76" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C76" s="8">
-        <v>0</v>
+      <c r="C76" s="16">
+        <v>1</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>90</v>
@@ -8169,17 +8190,17 @@
       <c r="Y76" s="5"/>
       <c r="Z76" s="5"/>
       <c r="AA76" s="5"/>
-      <c r="AB76" s="5" t="s">
+      <c r="AB76" s="8" t="s">
         <v>90</v>
       </c>
       <c r="AC76" s="5"/>
       <c r="AD76" s="5"/>
-      <c r="AE76" s="5" t="s">
+      <c r="AE76" s="8" t="s">
         <v>90</v>
       </c>
       <c r="AF76" s="5"/>
       <c r="AG76" s="5"/>
-      <c r="AH76" s="5" t="s">
+      <c r="AH76" s="8" t="s">
         <v>90</v>
       </c>
       <c r="AI76" s="5"/>
@@ -8205,52 +8226,52 @@
       <c r="A77" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C77" s="8">
-        <v>0</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>90</v>
+      <c r="C77" s="16">
+        <v>1</v>
+      </c>
+      <c r="D77" s="5">
+        <v>0</v>
+      </c>
+      <c r="E77" s="5">
+        <v>0</v>
+      </c>
+      <c r="F77" s="5">
+        <v>0</v>
+      </c>
+      <c r="G77" s="5">
+        <v>0</v>
+      </c>
+      <c r="H77" s="5">
+        <v>0</v>
       </c>
       <c r="I77" s="5"/>
       <c r="J77" s="5" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="K77" s="5" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="L77" s="5"/>
       <c r="M77" s="5"/>
       <c r="N77" s="5" t="s">
-        <v>90</v>
+        <v>165</v>
       </c>
       <c r="O77" s="5"/>
       <c r="P77" s="5" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="Q77" s="5"/>
       <c r="R77" s="5" t="s">
         <v>90</v>
       </c>
       <c r="S77" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="T77" s="5" t="s">
-        <v>90</v>
+        <v>30</v>
+      </c>
+      <c r="T77" s="5">
+        <v>0</v>
       </c>
       <c r="U77" s="17" t="s">
         <v>90</v>
@@ -8261,18 +8282,18 @@
       <c r="Y77" s="5"/>
       <c r="Z77" s="5"/>
       <c r="AA77" s="5"/>
-      <c r="AB77" s="5" t="s">
-        <v>90</v>
+      <c r="AB77" s="5">
+        <v>0</v>
       </c>
       <c r="AC77" s="5"/>
       <c r="AD77" s="5"/>
-      <c r="AE77" s="5" t="s">
-        <v>90</v>
+      <c r="AE77" s="5">
+        <v>0</v>
       </c>
       <c r="AF77" s="5"/>
       <c r="AG77" s="5"/>
-      <c r="AH77" s="5" t="s">
-        <v>90</v>
+      <c r="AH77" s="5">
+        <v>0</v>
       </c>
       <c r="AI77" s="5"/>
       <c r="AJ77" s="5"/>
@@ -8300,8 +8321,8 @@
       <c r="B78" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C78" s="8">
-        <v>0</v>
+      <c r="C78" s="16">
+        <v>1</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>90</v>
@@ -8481,55 +8502,55 @@
       <c r="A80" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C80" s="8">
-        <v>0</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H80" s="5" t="s">
-        <v>90</v>
+      <c r="C80" s="16">
+        <v>1</v>
+      </c>
+      <c r="D80" s="5">
+        <v>0</v>
+      </c>
+      <c r="E80" s="5">
+        <v>0</v>
+      </c>
+      <c r="F80" s="5">
+        <v>0</v>
+      </c>
+      <c r="G80" s="5">
+        <v>0</v>
+      </c>
+      <c r="H80" s="5">
+        <v>0</v>
       </c>
       <c r="I80" s="5"/>
       <c r="J80" s="5" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="K80" s="5" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="L80" s="5"/>
       <c r="M80" s="5"/>
       <c r="N80" s="5" t="s">
-        <v>90</v>
+        <v>165</v>
       </c>
       <c r="O80" s="5"/>
       <c r="P80" s="5" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="Q80" s="5"/>
       <c r="R80" s="5" t="s">
         <v>90</v>
       </c>
       <c r="S80" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="T80" s="5" t="s">
-        <v>90</v>
+        <v>30</v>
+      </c>
+      <c r="T80" s="5">
+        <v>1</v>
       </c>
       <c r="U80" s="17" t="s">
-        <v>90</v>
+        <v>183</v>
       </c>
       <c r="V80" s="5"/>
       <c r="W80" s="5"/>
@@ -8537,18 +8558,18 @@
       <c r="Y80" s="5"/>
       <c r="Z80" s="5"/>
       <c r="AA80" s="5"/>
-      <c r="AB80" s="5" t="s">
-        <v>90</v>
+      <c r="AB80" s="5">
+        <v>0</v>
       </c>
       <c r="AC80" s="5"/>
       <c r="AD80" s="5"/>
-      <c r="AE80" s="5" t="s">
-        <v>90</v>
+      <c r="AE80" s="5">
+        <v>0</v>
       </c>
       <c r="AF80" s="5"/>
       <c r="AG80" s="5"/>
-      <c r="AH80" s="5" t="s">
-        <v>90</v>
+      <c r="AH80" s="5">
+        <v>0</v>
       </c>
       <c r="AI80" s="5"/>
       <c r="AJ80" s="5"/>
@@ -8668,8 +8689,8 @@
       <c r="B82" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C82" s="8">
-        <v>0</v>
+      <c r="C82" s="16">
+        <v>1</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>90</v>
@@ -8849,55 +8870,55 @@
       <c r="A84" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C84" s="8">
-        <v>0</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G84" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H84" s="5" t="s">
-        <v>90</v>
+      <c r="C84" s="16">
+        <v>1</v>
+      </c>
+      <c r="D84" s="5">
+        <v>0</v>
+      </c>
+      <c r="E84" s="5">
+        <v>0</v>
+      </c>
+      <c r="F84" s="5">
+        <v>0</v>
+      </c>
+      <c r="G84" s="5">
+        <v>0</v>
+      </c>
+      <c r="H84" s="5">
+        <v>0</v>
       </c>
       <c r="I84" s="5"/>
       <c r="J84" s="5" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="K84" s="5" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="L84" s="5"/>
       <c r="M84" s="5"/>
       <c r="N84" s="5" t="s">
-        <v>90</v>
+        <v>165</v>
       </c>
       <c r="O84" s="5"/>
       <c r="P84" s="5" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="Q84" s="5"/>
       <c r="R84" s="5" t="s">
         <v>90</v>
       </c>
       <c r="S84" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="T84" s="5" t="s">
-        <v>90</v>
+        <v>30</v>
+      </c>
+      <c r="T84" s="5">
+        <v>1</v>
       </c>
       <c r="U84" s="17" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="V84" s="5"/>
       <c r="W84" s="5"/>
@@ -8905,18 +8926,18 @@
       <c r="Y84" s="5"/>
       <c r="Z84" s="5"/>
       <c r="AA84" s="5"/>
-      <c r="AB84" s="5" t="s">
-        <v>90</v>
+      <c r="AB84" s="5">
+        <v>0</v>
       </c>
       <c r="AC84" s="5"/>
       <c r="AD84" s="5"/>
-      <c r="AE84" s="5" t="s">
-        <v>90</v>
+      <c r="AE84" s="5">
+        <v>0</v>
       </c>
       <c r="AF84" s="5"/>
       <c r="AG84" s="5"/>
-      <c r="AH84" s="5" t="s">
-        <v>90</v>
+      <c r="AH84" s="5">
+        <v>0</v>
       </c>
       <c r="AI84" s="5"/>
       <c r="AJ84" s="5"/>
@@ -8944,7 +8965,7 @@
       <c r="B85" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C85" s="16">
+      <c r="C85" s="8">
         <v>0</v>
       </c>
       <c r="D85" s="5" t="s">
@@ -9031,6 +9052,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:R2"/>
     <mergeCell ref="AV2:AW2"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="Z1:AI1"/>
@@ -9043,11 +9069,6 @@
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AU2"/>
     <mergeCell ref="J1:X1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Raw ICA vs. ECG ICA
</commit_message>
<xml_diff>
--- a/meta/MEG_ANALYSIS_MASTERFILE.xlsx
+++ b/meta/MEG_ANALYSIS_MASTERFILE.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\meditation\ERC\Analyses\MEG\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565B6422-246D-4E37-81E2-49C5715C7D50}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF9FE97-C7F3-45C4-9A31-6D351394B18E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9435" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MEG_ANALYSIS_MASTERFILE" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3988" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="185">
   <si>
     <t>ANATOMY</t>
   </si>
@@ -1198,10 +1198,10 @@
   <dimension ref="A1:AZ83"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="F53" sqref="F53"/>
+      <selection pane="bottomRight" activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6224,23 +6224,23 @@
       <c r="B55" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="C55" s="15">
-        <v>0</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E55" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F55" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G55" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="H55" s="13" t="s">
-        <v>90</v>
+      <c r="C55" s="23">
+        <v>1</v>
+      </c>
+      <c r="D55" s="15">
+        <v>0</v>
+      </c>
+      <c r="E55" s="13">
+        <v>0</v>
+      </c>
+      <c r="F55" s="13">
+        <v>0</v>
+      </c>
+      <c r="G55" s="13">
+        <v>0</v>
+      </c>
+      <c r="H55" s="13">
+        <v>0</v>
       </c>
       <c r="I55" s="13"/>
       <c r="J55" s="5" t="s">
@@ -6316,23 +6316,23 @@
       <c r="B56" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C56" s="15">
-        <v>0</v>
-      </c>
-      <c r="D56" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E56" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F56" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G56" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="H56" s="13" t="s">
-        <v>90</v>
+      <c r="C56" s="23">
+        <v>1</v>
+      </c>
+      <c r="D56" s="15">
+        <v>0</v>
+      </c>
+      <c r="E56" s="13">
+        <v>0</v>
+      </c>
+      <c r="F56" s="13">
+        <v>0</v>
+      </c>
+      <c r="G56" s="13">
+        <v>0</v>
+      </c>
+      <c r="H56" s="13">
+        <v>0</v>
       </c>
       <c r="I56" s="13"/>
       <c r="J56" s="5" t="s">
@@ -6411,10 +6411,10 @@
       <c r="C57" s="23">
         <v>1</v>
       </c>
-      <c r="D57" s="15">
-        <v>0</v>
-      </c>
-      <c r="E57" s="13">
+      <c r="D57" s="23">
+        <v>1</v>
+      </c>
+      <c r="E57" s="15">
         <v>0</v>
       </c>
       <c r="F57" s="13">
@@ -6592,23 +6592,23 @@
       <c r="B59" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="C59" s="15">
-        <v>0</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F59" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G59" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="H59" s="13" t="s">
-        <v>90</v>
+      <c r="C59" s="23">
+        <v>1</v>
+      </c>
+      <c r="D59" s="15">
+        <v>0</v>
+      </c>
+      <c r="E59" s="13">
+        <v>0</v>
+      </c>
+      <c r="F59" s="13">
+        <v>0</v>
+      </c>
+      <c r="G59" s="13">
+        <v>0</v>
+      </c>
+      <c r="H59" s="13">
+        <v>0</v>
       </c>
       <c r="I59" s="13"/>
       <c r="J59" s="13" t="s">
@@ -6684,23 +6684,23 @@
       <c r="B60" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="C60" s="15">
-        <v>0</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E60" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F60" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G60" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="H60" s="13" t="s">
-        <v>90</v>
+      <c r="C60" s="23">
+        <v>1</v>
+      </c>
+      <c r="D60" s="15">
+        <v>0</v>
+      </c>
+      <c r="E60" s="13">
+        <v>0</v>
+      </c>
+      <c r="F60" s="13">
+        <v>0</v>
+      </c>
+      <c r="G60" s="13">
+        <v>0</v>
+      </c>
+      <c r="H60" s="13">
+        <v>0</v>
       </c>
       <c r="I60" s="13"/>
       <c r="J60" s="13" t="s">
@@ -6776,23 +6776,23 @@
       <c r="B61" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="C61" s="15">
-        <v>0</v>
-      </c>
-      <c r="D61" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E61" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F61" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G61" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="H61" s="13" t="s">
-        <v>90</v>
+      <c r="C61" s="23">
+        <v>1</v>
+      </c>
+      <c r="D61" s="15">
+        <v>0</v>
+      </c>
+      <c r="E61" s="13">
+        <v>0</v>
+      </c>
+      <c r="F61" s="13">
+        <v>0</v>
+      </c>
+      <c r="G61" s="13">
+        <v>0</v>
+      </c>
+      <c r="H61" s="13">
+        <v>0</v>
       </c>
       <c r="I61" s="13"/>
       <c r="J61" s="13" t="s">
@@ -7982,23 +7982,23 @@
       <c r="B74" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C74" s="8">
-        <v>0</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G74" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H74" s="5" t="s">
-        <v>90</v>
+      <c r="C74" s="16">
+        <v>1</v>
+      </c>
+      <c r="D74" s="8">
+        <v>0</v>
+      </c>
+      <c r="E74" s="5">
+        <v>0</v>
+      </c>
+      <c r="F74" s="5">
+        <v>0</v>
+      </c>
+      <c r="G74" s="5">
+        <v>0</v>
+      </c>
+      <c r="H74" s="5">
+        <v>0</v>
       </c>
       <c r="I74" s="5"/>
       <c r="J74" s="5" t="s">
@@ -8077,10 +8077,10 @@
       <c r="C75" s="16">
         <v>1</v>
       </c>
-      <c r="D75" s="8">
-        <v>0</v>
-      </c>
-      <c r="E75" s="5">
+      <c r="D75" s="16">
+        <v>1</v>
+      </c>
+      <c r="E75" s="8">
         <v>0</v>
       </c>
       <c r="F75" s="5">
@@ -8350,23 +8350,23 @@
       <c r="B78" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C78" s="8">
-        <v>0</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G78" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H78" s="5" t="s">
-        <v>90</v>
+      <c r="C78" s="16">
+        <v>1</v>
+      </c>
+      <c r="D78" s="8">
+        <v>0</v>
+      </c>
+      <c r="E78" s="5">
+        <v>0</v>
+      </c>
+      <c r="F78" s="5">
+        <v>0</v>
+      </c>
+      <c r="G78" s="5">
+        <v>0</v>
+      </c>
+      <c r="H78" s="5">
+        <v>0</v>
       </c>
       <c r="I78" s="5"/>
       <c r="J78" s="5" t="s">
@@ -8587,7 +8587,7 @@
       <c r="Y80" s="5"/>
       <c r="Z80" s="5"/>
       <c r="AA80" s="5"/>
-      <c r="AB80" s="5">
+      <c r="AB80" s="8">
         <v>0</v>
       </c>
       <c r="AC80" s="5"/>
@@ -8810,23 +8810,23 @@
       <c r="B83" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C83" s="8">
-        <v>0</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G83" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H83" s="5" t="s">
-        <v>90</v>
+      <c r="C83" s="16">
+        <v>1</v>
+      </c>
+      <c r="D83" s="8">
+        <v>0</v>
+      </c>
+      <c r="E83" s="5">
+        <v>0</v>
+      </c>
+      <c r="F83" s="5">
+        <v>0</v>
+      </c>
+      <c r="G83" s="5">
+        <v>0</v>
+      </c>
+      <c r="H83" s="5">
+        <v>0</v>
       </c>
       <c r="I83" s="5"/>
       <c r="J83" s="5" t="s">

</xml_diff>